<commit_message>
read excel in main
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -301,7 +301,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -482,16 +482,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -667,19 +667,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -861,13 +861,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1043,16 +1043,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>158</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1237,13 +1237,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>52</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>44</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1431,13 +1431,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1625,16 +1625,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>52</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1828,19 +1828,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2024,19 +2024,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2220,28 +2220,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2416,19 +2416,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>146</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2616,13 +2616,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2816,19 +2816,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3016,10 +3016,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3207,19 +3207,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -4210,7 +4210,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4296,7 +4296,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4304,7 +4304,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4312,7 +4312,7 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>51</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4320,7 +4320,7 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4366,7 +4366,7 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4374,7 +4374,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4382,7 +4382,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4390,7 +4390,7 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4398,7 +4398,7 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4460,7 +4460,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4468,7 +4468,7 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4476,7 +4476,7 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4514,7 +4514,7 @@
         <v>30</v>
       </c>
       <c r="B1">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4522,7 +4522,7 @@
         <v>31</v>
       </c>
       <c r="B2">
-        <v>158</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4530,7 +4530,7 @@
         <v>32</v>
       </c>
       <c r="B3">
-        <v>115</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4538,7 +4538,7 @@
         <v>33</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4600,7 +4600,7 @@
         <v>30</v>
       </c>
       <c r="B1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4608,7 +4608,7 @@
         <v>31</v>
       </c>
       <c r="B2">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4616,7 +4616,7 @@
         <v>32</v>
       </c>
       <c r="B3">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4686,7 +4686,7 @@
         <v>30</v>
       </c>
       <c r="B1">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4694,7 +4694,7 @@
         <v>31</v>
       </c>
       <c r="B2">
-        <v>62</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4702,7 +4702,7 @@
         <v>32</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4772,7 +4772,7 @@
         <v>30</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4780,7 +4780,7 @@
         <v>31</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4788,7 +4788,7 @@
         <v>32</v>
       </c>
       <c r="B3">
-        <v>52</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4796,7 +4796,7 @@
         <v>33</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4866,7 +4866,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4874,7 +4874,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4882,7 +4882,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4890,7 +4890,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4898,7 +4898,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4968,7 +4968,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>79</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4976,7 +4976,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4984,7 +4984,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4992,7 +4992,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5000,7 +5000,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5070,7 +5070,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5078,7 +5078,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5086,7 +5086,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5094,7 +5094,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5102,7 +5102,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5118,7 +5118,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5126,7 +5126,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5180,7 +5180,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>79</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5188,7 +5188,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>146</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5196,7 +5196,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5212,7 +5212,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5274,7 +5274,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5282,7 +5282,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>64</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5290,7 +5290,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5368,7 +5368,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5376,7 +5376,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5384,7 +5384,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5400,7 +5400,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5462,7 +5462,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5470,7 +5470,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5548,7 +5548,7 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5556,7 +5556,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5564,7 +5564,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>105</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5572,7 +5572,7 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>116</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5580,7 +5580,7 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>47</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">

</xml_diff>

<commit_message>
fixed so it shows better distribution
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="157">
   <si>
     <t>Deal Call Months</t>
   </si>
@@ -52,6 +52,9 @@
     <t>[37.0-38.0]</t>
   </si>
   <si>
+    <t>[38.0-38.0]</t>
+  </si>
+  <si>
     <t>[38.0-39.0]</t>
   </si>
   <si>
@@ -73,307 +76,430 @@
     <t>[44.0-45.0]</t>
   </si>
   <si>
-    <t>[45.0-46.0]</t>
-  </si>
-  <si>
-    <t>[38.0-38.0]</t>
-  </si>
-  <si>
-    <t>[3.5-3.6]</t>
-  </si>
-  <si>
-    <t>[3.6-3.7]</t>
-  </si>
-  <si>
-    <t>[3.7-3.8]</t>
-  </si>
-  <si>
-    <t>[3.8-3.9]</t>
-  </si>
-  <si>
-    <t>[3.9-3.9]</t>
-  </si>
-  <si>
-    <t>[3.9-4.0]</t>
-  </si>
-  <si>
-    <t>[4.0-4.1]</t>
-  </si>
-  <si>
-    <t>[4.1-4.2]</t>
-  </si>
-  <si>
-    <t>[4.2-4.2]</t>
-  </si>
-  <si>
-    <t>[4.2-4.3]</t>
-  </si>
-  <si>
-    <t>[4.3-4.4]</t>
-  </si>
-  <si>
-    <t>[4.4-4.5]</t>
-  </si>
-  <si>
-    <t>[4.5-4.6]</t>
-  </si>
-  <si>
-    <t>[4.6-4.6]</t>
-  </si>
-  <si>
-    <t>[3.8-3.8]</t>
-  </si>
-  <si>
-    <t>[6.6-6.9]</t>
-  </si>
-  <si>
-    <t>[6.9-7.3]</t>
-  </si>
-  <si>
-    <t>[7.3-7.6]</t>
-  </si>
-  <si>
-    <t>[7.6-7.9]</t>
-  </si>
-  <si>
-    <t>[7.9-8.2]</t>
-  </si>
-  <si>
-    <t>[8.2-8.6]</t>
-  </si>
-  <si>
-    <t>[8.6-8.9]</t>
-  </si>
-  <si>
-    <t>[8.9-9.2]</t>
-  </si>
-  <si>
-    <t>[9.2-9.5]</t>
-  </si>
-  <si>
-    <t>[9.5-9.9]</t>
-  </si>
-  <si>
-    <t>[9.9-10.2]</t>
-  </si>
-  <si>
-    <t>[10.2-10.5]</t>
-  </si>
-  <si>
-    <t>[10.5-10.8]</t>
-  </si>
-  <si>
-    <t>[10.8-11.2]</t>
-  </si>
-  <si>
-    <t>[6.9-7.2]</t>
-  </si>
-  <si>
-    <t>[7.2-7.6]</t>
-  </si>
-  <si>
-    <t>[8.2-8.5]</t>
-  </si>
-  <si>
-    <t>[8.5-8.9]</t>
-  </si>
-  <si>
-    <t>[9.5-9.8]</t>
-  </si>
-  <si>
-    <t>[9.8-10.1]</t>
-  </si>
-  <si>
-    <t>[10.1-10.5]</t>
-  </si>
-  <si>
-    <t>[10.8-11.1]</t>
-  </si>
-  <si>
-    <t>[6.6-7.0]</t>
-  </si>
-  <si>
-    <t>[7.0-7.3]</t>
-  </si>
-  <si>
-    <t>[6.7-7.0]</t>
-  </si>
-  <si>
-    <t>[7.9-8.3]</t>
-  </si>
-  <si>
-    <t>[8.3-8.6]</t>
-  </si>
-  <si>
-    <t>[9.2-9.6]</t>
-  </si>
-  <si>
-    <t>[9.6-9.9]</t>
-  </si>
-  <si>
-    <t>[0.6267-0.6563]</t>
-  </si>
-  <si>
-    <t>[0.6563-0.686]</t>
-  </si>
-  <si>
-    <t>[0.686-0.7156]</t>
-  </si>
-  <si>
-    <t>[0.7156-0.7453]</t>
-  </si>
-  <si>
-    <t>[0.7453-0.775]</t>
-  </si>
-  <si>
-    <t>[0.775-0.8046]</t>
-  </si>
-  <si>
-    <t>[0.8046-0.8343]</t>
-  </si>
-  <si>
-    <t>[0.8343-0.8639]</t>
-  </si>
-  <si>
-    <t>[0.8639-0.8936]</t>
-  </si>
-  <si>
-    <t>[0.8936-0.9232]</t>
-  </si>
-  <si>
-    <t>[0.9232-0.9529]</t>
-  </si>
-  <si>
-    <t>[0.9529-0.9825]</t>
-  </si>
-  <si>
-    <t>[0.9825-1.0122]</t>
-  </si>
-  <si>
-    <t>[1.0122-1.0418]</t>
-  </si>
-  <si>
-    <t>[0.6297-0.6591]</t>
-  </si>
-  <si>
-    <t>[0.6591-0.6885]</t>
-  </si>
-  <si>
-    <t>[0.6885-0.718]</t>
-  </si>
-  <si>
-    <t>[0.718-0.7474]</t>
-  </si>
-  <si>
-    <t>[0.7474-0.7769]</t>
-  </si>
-  <si>
-    <t>[0.7769-0.8063]</t>
-  </si>
-  <si>
-    <t>[0.8063-0.8358]</t>
-  </si>
-  <si>
-    <t>[0.8358-0.8652]</t>
-  </si>
-  <si>
-    <t>[0.8652-0.8946]</t>
-  </si>
-  <si>
-    <t>[0.8946-0.9241]</t>
-  </si>
-  <si>
-    <t>[0.9241-0.9535]</t>
-  </si>
-  <si>
-    <t>[0.9535-0.983]</t>
-  </si>
-  <si>
-    <t>[0.983-1.0124]</t>
-  </si>
-  <si>
-    <t>[1.0124-1.0418]</t>
-  </si>
-  <si>
-    <t>[0.6278-0.6574]</t>
-  </si>
-  <si>
-    <t>[0.6574-0.687]</t>
-  </si>
-  <si>
-    <t>[0.687-0.7165]</t>
-  </si>
-  <si>
-    <t>[0.7165-0.7461]</t>
-  </si>
-  <si>
-    <t>[0.7461-0.7757]</t>
-  </si>
-  <si>
-    <t>[0.7757-0.8052]</t>
-  </si>
-  <si>
-    <t>[0.8052-0.8348]</t>
-  </si>
-  <si>
-    <t>[0.8348-0.8644]</t>
-  </si>
-  <si>
-    <t>[0.8644-0.8939]</t>
-  </si>
-  <si>
-    <t>[0.8939-0.9235]</t>
-  </si>
-  <si>
-    <t>[0.9235-0.953]</t>
-  </si>
-  <si>
-    <t>[0.953-0.9826]</t>
-  </si>
-  <si>
-    <t>[0.9826-1.0122]</t>
-  </si>
-  <si>
-    <t>[1.0122-1.0417]</t>
-  </si>
-  <si>
-    <t>[0.6563-0.6859]</t>
-  </si>
-  <si>
-    <t>[0.6859-0.7155]</t>
-  </si>
-  <si>
-    <t>[0.7155-0.7451]</t>
-  </si>
-  <si>
-    <t>[0.7451-0.7747]</t>
-  </si>
-  <si>
-    <t>[0.7747-0.8044]</t>
-  </si>
-  <si>
-    <t>[0.8044-0.834]</t>
-  </si>
-  <si>
-    <t>[0.834-0.8636]</t>
-  </si>
-  <si>
-    <t>[0.8636-0.8932]</t>
-  </si>
-  <si>
-    <t>[0.8932-0.9228]</t>
-  </si>
-  <si>
-    <t>[0.9228-0.9524]</t>
-  </si>
-  <si>
-    <t>[0.9524-0.982]</t>
-  </si>
-  <si>
-    <t>[0.982-1.0116]</t>
-  </si>
-  <si>
-    <t>[1.0116-1.0413]</t>
+    <t>[36.0-36.0]</t>
+  </si>
+  <si>
+    <t>[42.0-42.0]</t>
+  </si>
+  <si>
+    <t>[3.9995-4.0108]</t>
+  </si>
+  <si>
+    <t>[4.0108-4.0221]</t>
+  </si>
+  <si>
+    <t>[4.0221-4.0334]</t>
+  </si>
+  <si>
+    <t>[4.0334-4.0446]</t>
+  </si>
+  <si>
+    <t>[4.0446-4.0559]</t>
+  </si>
+  <si>
+    <t>[4.0559-4.0672]</t>
+  </si>
+  <si>
+    <t>[4.0672-4.0785]</t>
+  </si>
+  <si>
+    <t>[4.0785-4.0897]</t>
+  </si>
+  <si>
+    <t>[4.0897-4.101]</t>
+  </si>
+  <si>
+    <t>[4.101-4.1123]</t>
+  </si>
+  <si>
+    <t>[4.1123-4.1236]</t>
+  </si>
+  <si>
+    <t>[4.1236-4.1348]</t>
+  </si>
+  <si>
+    <t>[4.1348-4.1461]</t>
+  </si>
+  <si>
+    <t>[4.1461-4.1574]</t>
+  </si>
+  <si>
+    <t>[4.0311-4.0398]</t>
+  </si>
+  <si>
+    <t>[4.0398-4.0486]</t>
+  </si>
+  <si>
+    <t>[4.0486-4.0573]</t>
+  </si>
+  <si>
+    <t>[4.0573-4.066]</t>
+  </si>
+  <si>
+    <t>[4.066-4.0747]</t>
+  </si>
+  <si>
+    <t>[4.0747-4.0834]</t>
+  </si>
+  <si>
+    <t>[4.0834-4.0922]</t>
+  </si>
+  <si>
+    <t>[4.0922-4.1009]</t>
+  </si>
+  <si>
+    <t>[4.1009-4.1096]</t>
+  </si>
+  <si>
+    <t>[4.1096-4.1183]</t>
+  </si>
+  <si>
+    <t>[4.1183-4.127]</t>
+  </si>
+  <si>
+    <t>[4.127-4.1358]</t>
+  </si>
+  <si>
+    <t>[4.1358-4.1445]</t>
+  </si>
+  <si>
+    <t>[4.1445-4.1532]</t>
+  </si>
+  <si>
+    <t>[4.0271-4.0352]</t>
+  </si>
+  <si>
+    <t>[4.0352-4.0433]</t>
+  </si>
+  <si>
+    <t>[4.0433-4.0513]</t>
+  </si>
+  <si>
+    <t>[4.0513-4.0594]</t>
+  </si>
+  <si>
+    <t>[4.0594-4.0674]</t>
+  </si>
+  <si>
+    <t>[4.0674-4.0755]</t>
+  </si>
+  <si>
+    <t>[4.0755-4.0836]</t>
+  </si>
+  <si>
+    <t>[4.0836-4.0916]</t>
+  </si>
+  <si>
+    <t>[4.0916-4.0997]</t>
+  </si>
+  <si>
+    <t>[4.0997-4.1077]</t>
+  </si>
+  <si>
+    <t>[4.1077-4.1158]</t>
+  </si>
+  <si>
+    <t>[4.1158-4.1239]</t>
+  </si>
+  <si>
+    <t>[4.1239-4.1319]</t>
+  </si>
+  <si>
+    <t>[4.1319-4.14]</t>
+  </si>
+  <si>
+    <t>[8.523-8.582]</t>
+  </si>
+  <si>
+    <t>[8.582-8.641]</t>
+  </si>
+  <si>
+    <t>[8.641-8.7]</t>
+  </si>
+  <si>
+    <t>[8.7-8.759]</t>
+  </si>
+  <si>
+    <t>[8.759-8.818]</t>
+  </si>
+  <si>
+    <t>[8.818-8.877]</t>
+  </si>
+  <si>
+    <t>[8.877-8.936]</t>
+  </si>
+  <si>
+    <t>[8.936-8.995]</t>
+  </si>
+  <si>
+    <t>[8.995-9.054]</t>
+  </si>
+  <si>
+    <t>[9.054-9.113]</t>
+  </si>
+  <si>
+    <t>[9.113-9.172]</t>
+  </si>
+  <si>
+    <t>[9.172-9.231]</t>
+  </si>
+  <si>
+    <t>[9.231-9.289]</t>
+  </si>
+  <si>
+    <t>[9.289-9.348]</t>
+  </si>
+  <si>
+    <t>[8.541-8.586]</t>
+  </si>
+  <si>
+    <t>[8.586-8.631]</t>
+  </si>
+  <si>
+    <t>[8.631-8.676]</t>
+  </si>
+  <si>
+    <t>[8.676-8.721]</t>
+  </si>
+  <si>
+    <t>[8.721-8.766]</t>
+  </si>
+  <si>
+    <t>[8.766-8.811]</t>
+  </si>
+  <si>
+    <t>[8.811-8.856]</t>
+  </si>
+  <si>
+    <t>[8.856-8.901]</t>
+  </si>
+  <si>
+    <t>[8.901-8.946]</t>
+  </si>
+  <si>
+    <t>[8.946-8.991]</t>
+  </si>
+  <si>
+    <t>[8.991-9.037]</t>
+  </si>
+  <si>
+    <t>[9.037-9.082]</t>
+  </si>
+  <si>
+    <t>[9.082-9.127]</t>
+  </si>
+  <si>
+    <t>[9.127-9.172]</t>
+  </si>
+  <si>
+    <t>[8.609-8.651]</t>
+  </si>
+  <si>
+    <t>[8.651-8.693]</t>
+  </si>
+  <si>
+    <t>[8.693-8.735]</t>
+  </si>
+  <si>
+    <t>[8.735-8.776]</t>
+  </si>
+  <si>
+    <t>[8.776-8.818]</t>
+  </si>
+  <si>
+    <t>[8.818-8.86]</t>
+  </si>
+  <si>
+    <t>[8.86-8.902]</t>
+  </si>
+  <si>
+    <t>[8.902-8.943]</t>
+  </si>
+  <si>
+    <t>[8.943-8.985]</t>
+  </si>
+  <si>
+    <t>[8.985-9.027]</t>
+  </si>
+  <si>
+    <t>[9.027-9.069]</t>
+  </si>
+  <si>
+    <t>[9.069-9.11]</t>
+  </si>
+  <si>
+    <t>[9.11-9.152]</t>
+  </si>
+  <si>
+    <t>[9.152-9.194]</t>
+  </si>
+  <si>
+    <t>[0.8268-0.828]</t>
+  </si>
+  <si>
+    <t>[0.828-0.8291]</t>
+  </si>
+  <si>
+    <t>[0.8291-0.8302]</t>
+  </si>
+  <si>
+    <t>[0.8302-0.8313]</t>
+  </si>
+  <si>
+    <t>[0.8313-0.8325]</t>
+  </si>
+  <si>
+    <t>[0.8325-0.8336]</t>
+  </si>
+  <si>
+    <t>[0.8336-0.8347]</t>
+  </si>
+  <si>
+    <t>[0.8347-0.8359]</t>
+  </si>
+  <si>
+    <t>[0.8359-0.837]</t>
+  </si>
+  <si>
+    <t>[0.837-0.8381]</t>
+  </si>
+  <si>
+    <t>[0.8381-0.8392]</t>
+  </si>
+  <si>
+    <t>[0.8392-0.8404]</t>
+  </si>
+  <si>
+    <t>[0.8404-0.8415]</t>
+  </si>
+  <si>
+    <t>[0.8415-0.8426]</t>
+  </si>
+  <si>
+    <t>[0.8286-0.8296]</t>
+  </si>
+  <si>
+    <t>[0.8296-0.8306]</t>
+  </si>
+  <si>
+    <t>[0.8306-0.8316]</t>
+  </si>
+  <si>
+    <t>[0.8316-0.8326]</t>
+  </si>
+  <si>
+    <t>[0.8326-0.8336]</t>
+  </si>
+  <si>
+    <t>[0.8336-0.8346]</t>
+  </si>
+  <si>
+    <t>[0.8346-0.8356]</t>
+  </si>
+  <si>
+    <t>[0.8356-0.8366]</t>
+  </si>
+  <si>
+    <t>[0.8366-0.8376]</t>
+  </si>
+  <si>
+    <t>[0.8376-0.8386]</t>
+  </si>
+  <si>
+    <t>[0.8386-0.8396]</t>
+  </si>
+  <si>
+    <t>[0.8396-0.8406]</t>
+  </si>
+  <si>
+    <t>[0.8406-0.8416]</t>
+  </si>
+  <si>
+    <t>[0.8416-0.8426]</t>
+  </si>
+  <si>
+    <t>[0.8282-0.8292]</t>
+  </si>
+  <si>
+    <t>[0.8292-0.8302]</t>
+  </si>
+  <si>
+    <t>[0.8302-0.8312]</t>
+  </si>
+  <si>
+    <t>[0.8312-0.8322]</t>
+  </si>
+  <si>
+    <t>[0.8322-0.8332]</t>
+  </si>
+  <si>
+    <t>[0.8332-0.8342]</t>
+  </si>
+  <si>
+    <t>[0.8342-0.8351]</t>
+  </si>
+  <si>
+    <t>[0.8351-0.8361]</t>
+  </si>
+  <si>
+    <t>[0.8361-0.8371]</t>
+  </si>
+  <si>
+    <t>[0.8371-0.8381]</t>
+  </si>
+  <si>
+    <t>[0.8381-0.8391]</t>
+  </si>
+  <si>
+    <t>[0.8391-0.8401]</t>
+  </si>
+  <si>
+    <t>[0.8401-0.8411]</t>
+  </si>
+  <si>
+    <t>[0.8411-0.8421]</t>
+  </si>
+  <si>
+    <t>[0.8268-0.8279]</t>
+  </si>
+  <si>
+    <t>[0.8279-0.829]</t>
+  </si>
+  <si>
+    <t>[0.829-0.8301]</t>
+  </si>
+  <si>
+    <t>[0.8301-0.8311]</t>
+  </si>
+  <si>
+    <t>[0.8311-0.8322]</t>
+  </si>
+  <si>
+    <t>[0.8322-0.8333]</t>
+  </si>
+  <si>
+    <t>[0.8333-0.8344]</t>
+  </si>
+  <si>
+    <t>[0.8344-0.8354]</t>
+  </si>
+  <si>
+    <t>[0.8354-0.8365]</t>
+  </si>
+  <si>
+    <t>[0.8365-0.8376]</t>
+  </si>
+  <si>
+    <t>[0.8376-0.8387]</t>
+  </si>
+  <si>
+    <t>[0.8387-0.8397]</t>
+  </si>
+  <si>
+    <t>[0.8397-0.8408]</t>
+  </si>
+  <si>
+    <t>[0.8408-0.8419]</t>
   </si>
 </sst>
 </file>
@@ -469,6 +595,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Deal Call Months'!$A$1:$A$15</c:f>
@@ -493,28 +622,28 @@
                   <c:v>[37.0-38.0]</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>[38.0-38.0]</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>[38.0-39.0]</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>[39.0-40.0]</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>[40.0-41.0]</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>[41.0-42.0]</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>[42.0-43.0]</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>[43.0-44.0]</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>[44.0-45.0]</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>[45.0-46.0]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -529,43 +658,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>19</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -683,52 +812,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Proj Equity Yield Base'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[6.6-6.9]</c:v>
+                  <c:v>[8.541-8.586]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[6.9-7.2]</c:v>
+                  <c:v>[8.586-8.631]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[7.2-7.6]</c:v>
+                  <c:v>[8.631-8.676]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[7.6-7.9]</c:v>
+                  <c:v>[8.676-8.721]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[7.9-8.2]</c:v>
+                  <c:v>[8.721-8.766]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[8.2-8.5]</c:v>
+                  <c:v>[8.766-8.811]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[8.5-8.9]</c:v>
+                  <c:v>[8.811-8.856]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[8.9-9.2]</c:v>
+                  <c:v>[8.856-8.901]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[9.2-9.5]</c:v>
+                  <c:v>[8.901-8.946]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[9.5-9.8]</c:v>
+                  <c:v>[8.946-8.991]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[9.8-10.1]</c:v>
+                  <c:v>[8.991-9.037]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[10.1-10.5]</c:v>
+                  <c:v>[9.037-9.082]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[10.5-10.8]</c:v>
+                  <c:v>[9.082-9.127]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[10.8-11.1]</c:v>
+                  <c:v>[9.127-9.172]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -743,40 +875,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -907,52 +1039,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Proj Equity Yield Downside'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[6.6-7.0]</c:v>
+                  <c:v>[8.523-8.582]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[7.0-7.3]</c:v>
+                  <c:v>[8.582-8.641]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[7.3-7.6]</c:v>
+                  <c:v>[8.641-8.7]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[7.6-7.9]</c:v>
+                  <c:v>[8.7-8.759]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[7.9-8.2]</c:v>
+                  <c:v>[8.759-8.818]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[8.2-8.6]</c:v>
+                  <c:v>[8.818-8.877]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[8.6-8.9]</c:v>
+                  <c:v>[8.877-8.936]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[8.9-9.2]</c:v>
+                  <c:v>[8.936-8.995]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[9.2-9.5]</c:v>
+                  <c:v>[8.995-9.054]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[9.5-9.9]</c:v>
+                  <c:v>[9.054-9.113]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[9.9-10.2]</c:v>
+                  <c:v>[9.113-9.172]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[10.2-10.5]</c:v>
+                  <c:v>[9.172-9.231]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[10.5-10.8]</c:v>
+                  <c:v>[9.231-9.289]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[10.8-11.1]</c:v>
+                  <c:v>[9.289-9.348]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -964,37 +1099,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>81</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -1003,7 +1138,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1131,52 +1266,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Proj Equity Yield Upside'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[6.7-7.0]</c:v>
+                  <c:v>[8.609-8.651]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[7.0-7.3]</c:v>
+                  <c:v>[8.651-8.693]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[7.3-7.6]</c:v>
+                  <c:v>[8.693-8.735]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[7.6-7.9]</c:v>
+                  <c:v>[8.735-8.776]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[7.9-8.3]</c:v>
+                  <c:v>[8.776-8.818]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[8.3-8.6]</c:v>
+                  <c:v>[8.818-8.86]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[8.6-8.9]</c:v>
+                  <c:v>[8.86-8.902]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[8.9-9.2]</c:v>
+                  <c:v>[8.902-8.943]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[9.2-9.6]</c:v>
+                  <c:v>[8.943-8.985]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[9.6-9.9]</c:v>
+                  <c:v>[8.985-9.027]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[9.9-10.2]</c:v>
+                  <c:v>[9.027-9.069]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[10.2-10.5]</c:v>
+                  <c:v>[9.069-9.11]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[10.5-10.8]</c:v>
+                  <c:v>[9.11-9.152]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[10.8-11.2]</c:v>
+                  <c:v>[9.152-9.194]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1191,40 +1329,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>66</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1355,52 +1493,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Adv Rate'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.6267-0.6563]</c:v>
+                  <c:v>[0.8268-0.828]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.6563-0.686]</c:v>
+                  <c:v>[0.828-0.8291]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.686-0.7156]</c:v>
+                  <c:v>[0.8291-0.8302]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.7156-0.7453]</c:v>
+                  <c:v>[0.8302-0.8313]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.7453-0.775]</c:v>
+                  <c:v>[0.8313-0.8325]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.775-0.8046]</c:v>
+                  <c:v>[0.8325-0.8336]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8046-0.8343]</c:v>
+                  <c:v>[0.8336-0.8347]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.8343-0.8639]</c:v>
+                  <c:v>[0.8347-0.8359]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8639-0.8936]</c:v>
+                  <c:v>[0.8359-0.837]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.8936-0.9232]</c:v>
+                  <c:v>[0.837-0.8381]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.9232-0.9529]</c:v>
+                  <c:v>[0.8381-0.8392]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.9529-0.9825]</c:v>
+                  <c:v>[0.8392-0.8404]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.9825-1.0122]</c:v>
+                  <c:v>[0.8404-0.8415]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[1.0122-1.0418]</c:v>
+                  <c:v>[0.8415-0.8426]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1412,46 +1553,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>253</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1579,52 +1720,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Adv Rate Base'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.6297-0.6591]</c:v>
+                  <c:v>[0.8286-0.8296]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.6591-0.6885]</c:v>
+                  <c:v>[0.8296-0.8306]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.6885-0.718]</c:v>
+                  <c:v>[0.8306-0.8316]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.718-0.7474]</c:v>
+                  <c:v>[0.8316-0.8326]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.7474-0.7769]</c:v>
+                  <c:v>[0.8326-0.8336]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.7769-0.8063]</c:v>
+                  <c:v>[0.8336-0.8346]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8063-0.8358]</c:v>
+                  <c:v>[0.8346-0.8356]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.8358-0.8652]</c:v>
+                  <c:v>[0.8356-0.8366]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8652-0.8946]</c:v>
+                  <c:v>[0.8366-0.8376]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.8946-0.9241]</c:v>
+                  <c:v>[0.8376-0.8386]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.9241-0.9535]</c:v>
+                  <c:v>[0.8386-0.8396]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.9535-0.983]</c:v>
+                  <c:v>[0.8396-0.8406]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.983-1.0124]</c:v>
+                  <c:v>[0.8406-0.8416]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[1.0124-1.0418]</c:v>
+                  <c:v>[0.8416-0.8426]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1636,46 +1780,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>85</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1803,52 +1947,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Adv Rate Downside'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.6278-0.6574]</c:v>
+                  <c:v>[0.8282-0.8292]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.6574-0.687]</c:v>
+                  <c:v>[0.8292-0.8302]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.687-0.7165]</c:v>
+                  <c:v>[0.8302-0.8312]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.7165-0.7461]</c:v>
+                  <c:v>[0.8312-0.8322]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.7461-0.7757]</c:v>
+                  <c:v>[0.8322-0.8332]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.7757-0.8052]</c:v>
+                  <c:v>[0.8332-0.8342]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8052-0.8348]</c:v>
+                  <c:v>[0.8342-0.8351]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.8348-0.8644]</c:v>
+                  <c:v>[0.8351-0.8361]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8644-0.8939]</c:v>
+                  <c:v>[0.8361-0.8371]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.8939-0.9235]</c:v>
+                  <c:v>[0.8371-0.8381]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.9235-0.953]</c:v>
+                  <c:v>[0.8381-0.8391]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.953-0.9826]</c:v>
+                  <c:v>[0.8391-0.8401]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.9826-1.0122]</c:v>
+                  <c:v>[0.8401-0.8411]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[1.0122-1.0417]</c:v>
+                  <c:v>[0.8411-0.8421]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1860,46 +2007,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2027,52 +2174,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Adv Rate Upside'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.6267-0.6563]</c:v>
+                  <c:v>[0.8268-0.8279]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.6563-0.6859]</c:v>
+                  <c:v>[0.8279-0.829]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.6859-0.7155]</c:v>
+                  <c:v>[0.829-0.8301]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.7155-0.7451]</c:v>
+                  <c:v>[0.8301-0.8311]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.7451-0.7747]</c:v>
+                  <c:v>[0.8311-0.8322]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.7747-0.8044]</c:v>
+                  <c:v>[0.8322-0.8333]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8044-0.834]</c:v>
+                  <c:v>[0.8333-0.8344]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.834-0.8636]</c:v>
+                  <c:v>[0.8344-0.8354]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8636-0.8932]</c:v>
+                  <c:v>[0.8354-0.8365]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.8932-0.9228]</c:v>
+                  <c:v>[0.8365-0.8376]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.9228-0.9524]</c:v>
+                  <c:v>[0.8376-0.8387]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.9524-0.982]</c:v>
+                  <c:v>[0.8387-0.8397]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.982-1.0116]</c:v>
+                  <c:v>[0.8397-0.8408]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[1.0116-1.0413]</c:v>
+                  <c:v>[0.8408-0.8419]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2084,46 +2234,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2251,22 +2401,25 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Deal Call Months Base'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[32.0-33.0]</c:v>
+                  <c:v>[33.0-34.0]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[33.0-34.0]</c:v>
+                  <c:v>[34.0-35.0]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[34.0-35.0]</c:v>
+                  <c:v>[35.0-36.0]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[35.0-36.0]</c:v>
+                  <c:v>[36.0-36.0]</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>[36.0-37.0]</c:v>
@@ -2275,19 +2428,19 @@
                   <c:v>[37.0-38.0]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[38.0-38.0]</c:v>
+                  <c:v>[38.0-39.0]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[38.0-39.0]</c:v>
+                  <c:v>[39.0-40.0]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[39.0-40.0]</c:v>
+                  <c:v>[40.0-41.0]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[40.0-41.0]</c:v>
+                  <c:v>[41.0-42.0]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[41.0-42.0]</c:v>
+                  <c:v>[42.0-42.0]</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>[42.0-43.0]</c:v>
@@ -2311,43 +2464,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2465,6 +2618,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Deal Call Months Downside'!$A$1:$A$15</c:f>
@@ -2489,28 +2645,28 @@
                   <c:v>[37.0-38.0]</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>[38.0-38.0]</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>[38.0-39.0]</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>[39.0-40.0]</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>[40.0-41.0]</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>[41.0-42.0]</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>[42.0-43.0]</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>[43.0-44.0]</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>[44.0-45.0]</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>[45.0-46.0]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2525,43 +2681,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2679,22 +2835,25 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Deal Call Months Upside'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[32.0-33.0]</c:v>
+                  <c:v>[33.0-34.0]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[33.0-34.0]</c:v>
+                  <c:v>[34.0-35.0]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[34.0-35.0]</c:v>
+                  <c:v>[35.0-36.0]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[35.0-36.0]</c:v>
+                  <c:v>[36.0-36.0]</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>[36.0-37.0]</c:v>
@@ -2715,16 +2874,16 @@
                   <c:v>[41.0-42.0]</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>[42.0-42.0]</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>[42.0-43.0]</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>[43.0-44.0]</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>[44.0-45.0]</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>[45.0-46.0]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2739,43 +2898,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2893,52 +3052,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Cost of Funds'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.5-3.6]</c:v>
+                  <c:v>[3.9995-4.0108]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.6-3.7]</c:v>
+                  <c:v>[4.0108-4.0221]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.7-3.8]</c:v>
+                  <c:v>[4.0221-4.0334]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.8-3.9]</c:v>
+                  <c:v>[4.0334-4.0446]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.9-3.9]</c:v>
+                  <c:v>[4.0446-4.0559]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9-4.0]</c:v>
+                  <c:v>[4.0559-4.0672]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.0-4.1]</c:v>
+                  <c:v>[4.0672-4.0785]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.1-4.2]</c:v>
+                  <c:v>[4.0785-4.0897]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.2-4.2]</c:v>
+                  <c:v>[4.0897-4.101]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.2-4.3]</c:v>
+                  <c:v>[4.101-4.1123]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.3-4.4]</c:v>
+                  <c:v>[4.1123-4.1236]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.4-4.5]</c:v>
+                  <c:v>[4.1236-4.1348]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.5-4.6]</c:v>
+                  <c:v>[4.1348-4.1461]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.6-4.6]</c:v>
+                  <c:v>[4.1461-4.1574]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2950,7 +3112,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2959,37 +3121,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>141</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>159</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3117,52 +3279,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Cost of Funds Base'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.5-3.6]</c:v>
+                  <c:v>[4.0311-4.0398]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.6-3.7]</c:v>
+                  <c:v>[4.0398-4.0486]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.7-3.8]</c:v>
+                  <c:v>[4.0486-4.0573]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.8-3.9]</c:v>
+                  <c:v>[4.0573-4.066]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.9-3.9]</c:v>
+                  <c:v>[4.066-4.0747]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9-4.0]</c:v>
+                  <c:v>[4.0747-4.0834]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.0-4.1]</c:v>
+                  <c:v>[4.0834-4.0922]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.1-4.2]</c:v>
+                  <c:v>[4.0922-4.1009]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.2-4.2]</c:v>
+                  <c:v>[4.1009-4.1096]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.2-4.3]</c:v>
+                  <c:v>[4.1096-4.1183]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.3-4.4]</c:v>
+                  <c:v>[4.1183-4.127]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.4-4.5]</c:v>
+                  <c:v>[4.127-4.1358]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.5-4.6]</c:v>
+                  <c:v>[4.1358-4.1445]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.6-4.6]</c:v>
+                  <c:v>[4.1445-4.1532]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3177,40 +3342,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -3341,52 +3506,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Cost of Funds Downside'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.5-3.6]</c:v>
+                  <c:v>[3.9995-4.0108]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.6-3.7]</c:v>
+                  <c:v>[4.0108-4.0221]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.7-3.8]</c:v>
+                  <c:v>[4.0221-4.0334]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.8-3.9]</c:v>
+                  <c:v>[4.0334-4.0446]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.9-3.9]</c:v>
+                  <c:v>[4.0446-4.0559]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9-4.0]</c:v>
+                  <c:v>[4.0559-4.0672]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.0-4.1]</c:v>
+                  <c:v>[4.0672-4.0785]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.1-4.2]</c:v>
+                  <c:v>[4.0785-4.0897]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.2-4.2]</c:v>
+                  <c:v>[4.0897-4.101]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.2-4.3]</c:v>
+                  <c:v>[4.101-4.1123]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.3-4.4]</c:v>
+                  <c:v>[4.1123-4.1236]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.4-4.5]</c:v>
+                  <c:v>[4.1236-4.1348]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.5-4.6]</c:v>
+                  <c:v>[4.1348-4.1461]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.6-4.6]</c:v>
+                  <c:v>[4.1461-4.1574]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3398,7 +3566,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3407,37 +3575,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3565,52 +3733,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'WA Cost of Funds Upside'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.5-3.6]</c:v>
+                  <c:v>[4.0271-4.0352]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.6-3.7]</c:v>
+                  <c:v>[4.0352-4.0433]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.7-3.8]</c:v>
+                  <c:v>[4.0433-4.0513]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.8-3.8]</c:v>
+                  <c:v>[4.0513-4.0594]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.8-3.9]</c:v>
+                  <c:v>[4.0594-4.0674]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9-4.0]</c:v>
+                  <c:v>[4.0674-4.0755]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.0-4.1]</c:v>
+                  <c:v>[4.0755-4.0836]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.1-4.2]</c:v>
+                  <c:v>[4.0836-4.0916]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.2-4.2]</c:v>
+                  <c:v>[4.0916-4.0997]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.2-4.3]</c:v>
+                  <c:v>[4.0997-4.1077]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.3-4.4]</c:v>
+                  <c:v>[4.1077-4.1158]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.4-4.5]</c:v>
+                  <c:v>[4.1158-4.1239]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.5-4.6]</c:v>
+                  <c:v>[4.1239-4.1319]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.6-4.6]</c:v>
+                  <c:v>[4.1319-4.14]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3625,40 +3796,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -3789,52 +3960,55 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
           <c:cat>
             <c:strRef>
               <c:f>'Proj Equity Yield'!$A$1:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[6.6-6.9]</c:v>
+                  <c:v>[8.523-8.582]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[6.9-7.3]</c:v>
+                  <c:v>[8.582-8.641]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[7.3-7.6]</c:v>
+                  <c:v>[8.641-8.7]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[7.6-7.9]</c:v>
+                  <c:v>[8.7-8.759]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[7.9-8.2]</c:v>
+                  <c:v>[8.759-8.818]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[8.2-8.6]</c:v>
+                  <c:v>[8.818-8.877]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[8.6-8.9]</c:v>
+                  <c:v>[8.877-8.936]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[8.9-9.2]</c:v>
+                  <c:v>[8.936-8.995]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[9.2-9.5]</c:v>
+                  <c:v>[8.995-9.054]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[9.5-9.9]</c:v>
+                  <c:v>[9.054-9.113]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[9.9-10.2]</c:v>
+                  <c:v>[9.113-9.172]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[10.2-10.5]</c:v>
+                  <c:v>[9.172-9.231]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[10.5-10.8]</c:v>
+                  <c:v>[9.231-9.289]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[10.8-11.2]</c:v>
+                  <c:v>[9.289-9.348]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3846,37 +4020,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>234</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>65</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3885,7 +4059,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4846,7 +5020,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4854,7 +5028,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4862,7 +5036,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4870,7 +5044,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4878,7 +5052,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4886,7 +5060,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4894,7 +5068,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4902,7 +5076,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4910,7 +5084,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4918,7 +5092,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4926,7 +5100,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4934,7 +5108,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4942,7 +5116,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4961,7 +5135,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -4969,103 +5143,103 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B7">
-        <v>88</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -5087,95 +5261,95 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B7">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -5183,7 +5357,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5191,10 +5365,10 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5213,7 +5387,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5221,103 +5395,103 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="B7">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B8">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -5339,114 +5513,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="B7">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="B8">
-        <v>253</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5465,114 +5639,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="B8">
-        <v>85</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5591,114 +5765,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="B8">
-        <v>85</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5717,15 +5891,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>143</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5733,98 +5907,98 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="B7">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="B8">
-        <v>77</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5843,7 +6017,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5851,26 +6025,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5878,7 +6052,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5886,71 +6060,71 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5980,7 +6154,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5988,7 +6162,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5996,7 +6170,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6012,7 +6186,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6020,7 +6194,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6028,7 +6202,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6036,7 +6210,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6044,7 +6218,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6060,7 +6234,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6068,7 +6242,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6076,7 +6250,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6095,7 +6269,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6103,26 +6277,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6130,7 +6304,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6138,36 +6312,36 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -6175,10 +6349,10 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6186,7 +6360,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6194,7 +6368,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6202,7 +6376,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6221,15 +6395,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6237,7 +6411,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6245,90 +6419,90 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>141</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>159</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6347,7 +6521,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6355,103 +6529,103 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B7">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B8">
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -6473,15 +6647,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6489,7 +6663,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6497,90 +6671,90 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>48</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
         <v>24</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
         <v>25</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6599,7 +6773,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6607,103 +6781,103 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -6725,95 +6899,95 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B7">
-        <v>234</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B8">
-        <v>65</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6821,7 +6995,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6829,10 +7003,10 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added market aware to spreadsheet, fixed waar percent
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -29,567 +29,564 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="186">
   <si>
     <t>Deal Call Months</t>
   </si>
   <si>
+    <t>[23.0-24.0]</t>
+  </si>
+  <si>
+    <t>[24.0-24.0]</t>
+  </si>
+  <si>
     <t>[24.0-25.0]</t>
   </si>
   <si>
+    <t>[25.0-26.0]</t>
+  </si>
+  <si>
+    <t>[26.0-26.0]</t>
+  </si>
+  <si>
+    <t>[26.0-27.0]</t>
+  </si>
+  <si>
+    <t>[27.0-28.0]</t>
+  </si>
+  <si>
+    <t>[28.0-28.0]</t>
+  </si>
+  <si>
+    <t>[28.0-29.0]</t>
+  </si>
+  <si>
+    <t>[29.0-29.0]</t>
+  </si>
+  <si>
+    <t>[29.0-30.0]</t>
+  </si>
+  <si>
+    <t>[30.0-31.0]</t>
+  </si>
+  <si>
+    <t>[31.0-31.0]</t>
+  </si>
+  <si>
+    <t>[31.0-32.0]</t>
+  </si>
+  <si>
     <t>[25.0-25.0]</t>
   </si>
   <si>
-    <t>[25.0-26.0]</t>
-  </si>
-  <si>
-    <t>[26.0-27.0]</t>
-  </si>
-  <si>
-    <t>[27.0-28.0]</t>
-  </si>
-  <si>
-    <t>[28.0-28.0]</t>
-  </si>
-  <si>
-    <t>[28.0-29.0]</t>
-  </si>
-  <si>
-    <t>[29.0-30.0]</t>
-  </si>
-  <si>
     <t>[30.0-30.0]</t>
   </si>
   <si>
-    <t>[30.0-31.0]</t>
-  </si>
-  <si>
-    <t>[31.0-32.0]</t>
-  </si>
-  <si>
-    <t>[32.0-33.0]</t>
-  </si>
-  <si>
-    <t>[33.0-33.0]</t>
-  </si>
-  <si>
-    <t>[33.0-34.0]</t>
-  </si>
-  <si>
-    <t>[24.0-24.0]</t>
-  </si>
-  <si>
-    <t>[26.0-26.0]</t>
-  </si>
-  <si>
     <t>[27.0-27.0]</t>
   </si>
   <si>
-    <t>[29.0-29.0]</t>
-  </si>
-  <si>
-    <t>[3.8214-3.8416]</t>
-  </si>
-  <si>
-    <t>[3.8416-3.8618]</t>
-  </si>
-  <si>
-    <t>[3.8618-3.882]</t>
-  </si>
-  <si>
-    <t>[3.882-3.9022]</t>
-  </si>
-  <si>
-    <t>[3.9022-3.9225]</t>
-  </si>
-  <si>
-    <t>[3.9225-3.9427]</t>
-  </si>
-  <si>
-    <t>[3.9427-3.9629]</t>
-  </si>
-  <si>
-    <t>[3.9629-3.9831]</t>
-  </si>
-  <si>
-    <t>[3.9831-4.0033]</t>
-  </si>
-  <si>
-    <t>[4.0033-4.0235]</t>
-  </si>
-  <si>
-    <t>[4.0235-4.0438]</t>
-  </si>
-  <si>
-    <t>[4.0438-4.064]</t>
-  </si>
-  <si>
-    <t>[4.064-4.0842]</t>
-  </si>
-  <si>
-    <t>[4.0842-4.1044]</t>
-  </si>
-  <si>
-    <t>[3.8247-3.8381]</t>
-  </si>
-  <si>
-    <t>[3.8381-3.8515]</t>
-  </si>
-  <si>
-    <t>[3.8515-3.865]</t>
-  </si>
-  <si>
-    <t>[3.865-3.8784]</t>
-  </si>
-  <si>
-    <t>[3.8784-3.8918]</t>
-  </si>
-  <si>
-    <t>[3.8918-3.9052]</t>
-  </si>
-  <si>
-    <t>[3.9052-3.9187]</t>
-  </si>
-  <si>
-    <t>[3.9187-3.9321]</t>
-  </si>
-  <si>
-    <t>[3.9321-3.9455]</t>
-  </si>
-  <si>
-    <t>[3.9455-3.959]</t>
-  </si>
-  <si>
-    <t>[3.959-3.9724]</t>
-  </si>
-  <si>
-    <t>[3.9724-3.9858]</t>
-  </si>
-  <si>
-    <t>[3.9858-3.9993]</t>
-  </si>
-  <si>
-    <t>[3.9993-4.0127]</t>
-  </si>
-  <si>
-    <t>[3.8941-3.9091]</t>
-  </si>
-  <si>
-    <t>[3.9091-3.9242]</t>
-  </si>
-  <si>
-    <t>[3.9242-3.9392]</t>
-  </si>
-  <si>
-    <t>[3.9392-3.9542]</t>
-  </si>
-  <si>
-    <t>[3.9542-3.9692]</t>
-  </si>
-  <si>
-    <t>[3.9692-3.9842]</t>
-  </si>
-  <si>
-    <t>[3.9842-3.9993]</t>
-  </si>
-  <si>
-    <t>[3.9993-4.0143]</t>
-  </si>
-  <si>
-    <t>[4.0143-4.0293]</t>
-  </si>
-  <si>
-    <t>[4.0293-4.0443]</t>
-  </si>
-  <si>
-    <t>[4.0443-4.0594]</t>
-  </si>
-  <si>
-    <t>[4.0594-4.0744]</t>
-  </si>
-  <si>
-    <t>[4.0744-4.0894]</t>
-  </si>
-  <si>
-    <t>[4.0894-4.1044]</t>
-  </si>
-  <si>
-    <t>[3.8214-3.8297]</t>
-  </si>
-  <si>
-    <t>[3.8297-3.838]</t>
-  </si>
-  <si>
-    <t>[3.838-3.8463]</t>
-  </si>
-  <si>
-    <t>[3.8463-3.8547]</t>
-  </si>
-  <si>
-    <t>[3.8547-3.863]</t>
-  </si>
-  <si>
-    <t>[3.863-3.8713]</t>
-  </si>
-  <si>
-    <t>[3.8713-3.8796]</t>
-  </si>
-  <si>
-    <t>[3.8796-3.8879]</t>
-  </si>
-  <si>
-    <t>[3.8879-3.8962]</t>
-  </si>
-  <si>
-    <t>[3.8962-3.9046]</t>
-  </si>
-  <si>
-    <t>[3.9046-3.9129]</t>
-  </si>
-  <si>
-    <t>[3.9129-3.9212]</t>
-  </si>
-  <si>
-    <t>[3.9212-3.9295]</t>
-  </si>
-  <si>
-    <t>[3.9295-3.9378]</t>
-  </si>
-  <si>
-    <t>[9.894-10.013]</t>
-  </si>
-  <si>
-    <t>[10.013-10.132]</t>
-  </si>
-  <si>
-    <t>[10.132-10.251]</t>
-  </si>
-  <si>
-    <t>[10.251-10.371]</t>
-  </si>
-  <si>
-    <t>[10.371-10.49]</t>
-  </si>
-  <si>
-    <t>[10.49-10.609]</t>
-  </si>
-  <si>
-    <t>[10.609-10.728]</t>
-  </si>
-  <si>
-    <t>[10.728-10.848]</t>
-  </si>
-  <si>
-    <t>[10.848-10.967]</t>
-  </si>
-  <si>
-    <t>[10.967-11.086]</t>
-  </si>
-  <si>
-    <t>[11.086-11.205]</t>
-  </si>
-  <si>
-    <t>[11.205-11.325]</t>
-  </si>
-  <si>
-    <t>[11.325-11.444]</t>
-  </si>
-  <si>
-    <t>[11.444-11.563]</t>
-  </si>
-  <si>
-    <t>[10.442-10.521]</t>
-  </si>
-  <si>
-    <t>[10.521-10.601]</t>
-  </si>
-  <si>
-    <t>[10.601-10.681]</t>
-  </si>
-  <si>
-    <t>[10.681-10.761]</t>
-  </si>
-  <si>
-    <t>[10.761-10.84]</t>
-  </si>
-  <si>
-    <t>[10.84-10.92]</t>
-  </si>
-  <si>
-    <t>[10.92-11.0]</t>
-  </si>
-  <si>
-    <t>[11.0-11.079]</t>
-  </si>
-  <si>
-    <t>[11.079-11.159]</t>
-  </si>
-  <si>
-    <t>[11.159-11.239]</t>
-  </si>
-  <si>
-    <t>[11.239-11.319]</t>
-  </si>
-  <si>
-    <t>[11.319-11.398]</t>
-  </si>
-  <si>
-    <t>[11.398-11.478]</t>
-  </si>
-  <si>
-    <t>[11.478-11.558]</t>
-  </si>
-  <si>
-    <t>[9.894-9.983]</t>
-  </si>
-  <si>
-    <t>[9.983-10.072]</t>
-  </si>
-  <si>
-    <t>[10.072-10.162]</t>
-  </si>
-  <si>
-    <t>[10.162-10.251]</t>
-  </si>
-  <si>
-    <t>[10.251-10.34]</t>
-  </si>
-  <si>
-    <t>[10.34-10.429]</t>
-  </si>
-  <si>
-    <t>[10.429-10.519]</t>
-  </si>
-  <si>
-    <t>[10.519-10.608]</t>
-  </si>
-  <si>
-    <t>[10.608-10.697]</t>
-  </si>
-  <si>
-    <t>[10.697-10.787]</t>
-  </si>
-  <si>
-    <t>[10.787-10.876]</t>
-  </si>
-  <si>
-    <t>[10.876-10.965]</t>
-  </si>
-  <si>
-    <t>[10.965-11.055]</t>
-  </si>
-  <si>
-    <t>[11.055-11.144]</t>
-  </si>
-  <si>
-    <t>[10.906-10.953]</t>
-  </si>
-  <si>
-    <t>[10.953-11.0]</t>
-  </si>
-  <si>
-    <t>[11.0-11.047]</t>
-  </si>
-  <si>
-    <t>[11.047-11.094]</t>
-  </si>
-  <si>
-    <t>[11.094-11.141]</t>
-  </si>
-  <si>
-    <t>[11.141-11.188]</t>
-  </si>
-  <si>
-    <t>[11.188-11.235]</t>
-  </si>
-  <si>
-    <t>[11.235-11.282]</t>
-  </si>
-  <si>
-    <t>[11.282-11.329]</t>
-  </si>
-  <si>
-    <t>[11.329-11.376]</t>
-  </si>
-  <si>
-    <t>[11.376-11.422]</t>
-  </si>
-  <si>
-    <t>[11.422-11.469]</t>
-  </si>
-  <si>
-    <t>[11.469-11.516]</t>
-  </si>
-  <si>
-    <t>[11.516-11.563]</t>
-  </si>
-  <si>
-    <t>[0.8352-0.8363]</t>
-  </si>
-  <si>
-    <t>[0.8363-0.8374]</t>
-  </si>
-  <si>
-    <t>[0.8374-0.8385]</t>
-  </si>
-  <si>
-    <t>[0.8385-0.8395]</t>
-  </si>
-  <si>
-    <t>[0.8395-0.8406]</t>
-  </si>
-  <si>
-    <t>[0.8406-0.8417]</t>
-  </si>
-  <si>
-    <t>[0.8417-0.8428]</t>
-  </si>
-  <si>
-    <t>[0.8428-0.8439]</t>
-  </si>
-  <si>
-    <t>[0.8439-0.845]</t>
-  </si>
-  <si>
-    <t>[0.845-0.8461]</t>
-  </si>
-  <si>
-    <t>[0.8461-0.8472]</t>
-  </si>
-  <si>
-    <t>[0.8472-0.8483]</t>
-  </si>
-  <si>
-    <t>[0.8483-0.8494]</t>
-  </si>
-  <si>
-    <t>[0.8494-0.8505]</t>
-  </si>
-  <si>
-    <t>[0.8387-0.8393]</t>
-  </si>
-  <si>
-    <t>[0.8393-0.8399]</t>
-  </si>
-  <si>
-    <t>[0.8399-0.8406]</t>
-  </si>
-  <si>
-    <t>[0.8406-0.8412]</t>
-  </si>
-  <si>
-    <t>[0.8412-0.8418]</t>
-  </si>
-  <si>
-    <t>[0.8418-0.8424]</t>
-  </si>
-  <si>
-    <t>[0.8424-0.8431]</t>
-  </si>
-  <si>
-    <t>[0.8431-0.8437]</t>
-  </si>
-  <si>
-    <t>[0.8437-0.8443]</t>
-  </si>
-  <si>
-    <t>[0.8443-0.8449]</t>
-  </si>
-  <si>
-    <t>[0.8449-0.8456]</t>
-  </si>
-  <si>
-    <t>[0.8456-0.8462]</t>
-  </si>
-  <si>
-    <t>[0.8462-0.8468]</t>
-  </si>
-  <si>
-    <t>[0.8468-0.8475]</t>
-  </si>
-  <si>
-    <t>[0.8352-0.8361]</t>
-  </si>
-  <si>
-    <t>[0.8361-0.8369]</t>
-  </si>
-  <si>
-    <t>[0.8369-0.8378]</t>
-  </si>
-  <si>
-    <t>[0.8378-0.8387]</t>
-  </si>
-  <si>
-    <t>[0.8387-0.8396]</t>
-  </si>
-  <si>
-    <t>[0.8396-0.8405]</t>
-  </si>
-  <si>
-    <t>[0.8405-0.8414]</t>
-  </si>
-  <si>
-    <t>[0.8414-0.8423]</t>
-  </si>
-  <si>
-    <t>[0.8423-0.8432]</t>
-  </si>
-  <si>
-    <t>[0.8432-0.844]</t>
-  </si>
-  <si>
-    <t>[0.844-0.8449]</t>
-  </si>
-  <si>
-    <t>[0.8449-0.8458]</t>
-  </si>
-  <si>
-    <t>[0.8458-0.8467]</t>
-  </si>
-  <si>
-    <t>[0.8467-0.8476]</t>
-  </si>
-  <si>
-    <t>[0.8366-0.8376]</t>
-  </si>
-  <si>
-    <t>[0.8376-0.8386]</t>
-  </si>
-  <si>
-    <t>[0.8386-0.8396]</t>
-  </si>
-  <si>
-    <t>[0.8396-0.8406]</t>
-  </si>
-  <si>
-    <t>[0.8406-0.8416]</t>
-  </si>
-  <si>
-    <t>[0.8416-0.8426]</t>
-  </si>
-  <si>
-    <t>[0.8426-0.8435]</t>
-  </si>
-  <si>
-    <t>[0.8435-0.8445]</t>
-  </si>
-  <si>
-    <t>[0.8445-0.8455]</t>
-  </si>
-  <si>
-    <t>[0.8455-0.8465]</t>
-  </si>
-  <si>
-    <t>[0.8465-0.8475]</t>
-  </si>
-  <si>
-    <t>[0.8475-0.8485]</t>
-  </si>
-  <si>
-    <t>[0.8485-0.8495]</t>
-  </si>
-  <si>
-    <t>[0.8495-0.8505]</t>
+    <t>[3.8313-3.8516]</t>
+  </si>
+  <si>
+    <t>[3.8516-3.8718]</t>
+  </si>
+  <si>
+    <t>[3.8718-3.8921]</t>
+  </si>
+  <si>
+    <t>[3.8921-3.9123]</t>
+  </si>
+  <si>
+    <t>[3.9123-3.9326]</t>
+  </si>
+  <si>
+    <t>[3.9326-3.9528]</t>
+  </si>
+  <si>
+    <t>[3.9528-3.9731]</t>
+  </si>
+  <si>
+    <t>[3.9731-3.9933]</t>
+  </si>
+  <si>
+    <t>[3.9933-4.0136]</t>
+  </si>
+  <si>
+    <t>[4.0136-4.0338]</t>
+  </si>
+  <si>
+    <t>[4.0338-4.0541]</t>
+  </si>
+  <si>
+    <t>[4.0541-4.0743]</t>
+  </si>
+  <si>
+    <t>[4.0743-4.0946]</t>
+  </si>
+  <si>
+    <t>[4.0946-4.1148]</t>
+  </si>
+  <si>
+    <t>[3.8313-3.8464]</t>
+  </si>
+  <si>
+    <t>[3.8464-3.8614]</t>
+  </si>
+  <si>
+    <t>[3.8614-3.8765]</t>
+  </si>
+  <si>
+    <t>[3.8765-3.8915]</t>
+  </si>
+  <si>
+    <t>[3.8915-3.9066]</t>
+  </si>
+  <si>
+    <t>[3.9066-3.9216]</t>
+  </si>
+  <si>
+    <t>[3.9216-3.9367]</t>
+  </si>
+  <si>
+    <t>[3.9367-3.9517]</t>
+  </si>
+  <si>
+    <t>[3.9517-3.9668]</t>
+  </si>
+  <si>
+    <t>[3.9668-3.9818]</t>
+  </si>
+  <si>
+    <t>[3.9818-3.9969]</t>
+  </si>
+  <si>
+    <t>[3.9969-4.0119]</t>
+  </si>
+  <si>
+    <t>[4.0119-4.027]</t>
+  </si>
+  <si>
+    <t>[4.027-4.042]</t>
+  </si>
+  <si>
+    <t>[3.9146-3.9289]</t>
+  </si>
+  <si>
+    <t>[3.9289-3.9432]</t>
+  </si>
+  <si>
+    <t>[3.9432-3.9575]</t>
+  </si>
+  <si>
+    <t>[3.9575-3.9718]</t>
+  </si>
+  <si>
+    <t>[3.9718-3.9861]</t>
+  </si>
+  <si>
+    <t>[3.9861-4.0004]</t>
+  </si>
+  <si>
+    <t>[4.0004-4.0147]</t>
+  </si>
+  <si>
+    <t>[4.0147-4.029]</t>
+  </si>
+  <si>
+    <t>[4.029-4.0433]</t>
+  </si>
+  <si>
+    <t>[4.0433-4.0576]</t>
+  </si>
+  <si>
+    <t>[4.0576-4.0719]</t>
+  </si>
+  <si>
+    <t>[4.0719-4.0862]</t>
+  </si>
+  <si>
+    <t>[4.0862-4.1005]</t>
+  </si>
+  <si>
+    <t>[4.1005-4.1148]</t>
+  </si>
+  <si>
+    <t>[3.8347-3.8449]</t>
+  </si>
+  <si>
+    <t>[3.8449-3.8551]</t>
+  </si>
+  <si>
+    <t>[3.8551-3.8653]</t>
+  </si>
+  <si>
+    <t>[3.8653-3.8755]</t>
+  </si>
+  <si>
+    <t>[3.8755-3.8857]</t>
+  </si>
+  <si>
+    <t>[3.8857-3.8959]</t>
+  </si>
+  <si>
+    <t>[3.8959-3.9061]</t>
+  </si>
+  <si>
+    <t>[3.9061-3.9163]</t>
+  </si>
+  <si>
+    <t>[3.9163-3.9265]</t>
+  </si>
+  <si>
+    <t>[3.9265-3.9367]</t>
+  </si>
+  <si>
+    <t>[3.9367-3.9469]</t>
+  </si>
+  <si>
+    <t>[3.9469-3.9571]</t>
+  </si>
+  <si>
+    <t>[3.9571-3.9673]</t>
+  </si>
+  <si>
+    <t>[3.9673-3.9775]</t>
+  </si>
+  <si>
+    <t>[9.829-9.95]</t>
+  </si>
+  <si>
+    <t>[9.95-10.07]</t>
+  </si>
+  <si>
+    <t>[10.07-10.191]</t>
+  </si>
+  <si>
+    <t>[10.191-10.311]</t>
+  </si>
+  <si>
+    <t>[10.311-10.432]</t>
+  </si>
+  <si>
+    <t>[10.432-10.552]</t>
+  </si>
+  <si>
+    <t>[10.552-10.673]</t>
+  </si>
+  <si>
+    <t>[10.673-10.793]</t>
+  </si>
+  <si>
+    <t>[10.793-10.914]</t>
+  </si>
+  <si>
+    <t>[10.914-11.034]</t>
+  </si>
+  <si>
+    <t>[11.034-11.155]</t>
+  </si>
+  <si>
+    <t>[11.155-11.276]</t>
+  </si>
+  <si>
+    <t>[11.276-11.396]</t>
+  </si>
+  <si>
+    <t>[11.396-11.517]</t>
+  </si>
+  <si>
+    <t>[10.26-10.349]</t>
+  </si>
+  <si>
+    <t>[10.349-10.439]</t>
+  </si>
+  <si>
+    <t>[10.439-10.529]</t>
+  </si>
+  <si>
+    <t>[10.529-10.619]</t>
+  </si>
+  <si>
+    <t>[10.619-10.709]</t>
+  </si>
+  <si>
+    <t>[10.709-10.798]</t>
+  </si>
+  <si>
+    <t>[10.798-10.888]</t>
+  </si>
+  <si>
+    <t>[10.888-10.978]</t>
+  </si>
+  <si>
+    <t>[10.978-11.068]</t>
+  </si>
+  <si>
+    <t>[11.068-11.157]</t>
+  </si>
+  <si>
+    <t>[11.157-11.247]</t>
+  </si>
+  <si>
+    <t>[11.247-11.337]</t>
+  </si>
+  <si>
+    <t>[11.337-11.427]</t>
+  </si>
+  <si>
+    <t>[11.427-11.517]</t>
+  </si>
+  <si>
+    <t>[9.829-9.916]</t>
+  </si>
+  <si>
+    <t>[9.916-10.003]</t>
+  </si>
+  <si>
+    <t>[10.003-10.09]</t>
+  </si>
+  <si>
+    <t>[10.09-10.177]</t>
+  </si>
+  <si>
+    <t>[10.177-10.264]</t>
+  </si>
+  <si>
+    <t>[10.264-10.351]</t>
+  </si>
+  <si>
+    <t>[10.351-10.438]</t>
+  </si>
+  <si>
+    <t>[10.438-10.526]</t>
+  </si>
+  <si>
+    <t>[10.526-10.613]</t>
+  </si>
+  <si>
+    <t>[10.613-10.7]</t>
+  </si>
+  <si>
+    <t>[10.7-10.787]</t>
+  </si>
+  <si>
+    <t>[10.787-10.874]</t>
+  </si>
+  <si>
+    <t>[10.874-10.961]</t>
+  </si>
+  <si>
+    <t>[10.961-11.048]</t>
+  </si>
+  <si>
+    <t>[10.65-10.71]</t>
+  </si>
+  <si>
+    <t>[10.71-10.77]</t>
+  </si>
+  <si>
+    <t>[10.77-10.83]</t>
+  </si>
+  <si>
+    <t>[10.83-10.89]</t>
+  </si>
+  <si>
+    <t>[10.89-10.949]</t>
+  </si>
+  <si>
+    <t>[10.949-11.009]</t>
+  </si>
+  <si>
+    <t>[11.009-11.069]</t>
+  </si>
+  <si>
+    <t>[11.069-11.129]</t>
+  </si>
+  <si>
+    <t>[11.129-11.189]</t>
+  </si>
+  <si>
+    <t>[11.189-11.248]</t>
+  </si>
+  <si>
+    <t>[11.248-11.308]</t>
+  </si>
+  <si>
+    <t>[11.308-11.368]</t>
+  </si>
+  <si>
+    <t>[11.368-11.428]</t>
+  </si>
+  <si>
+    <t>[11.428-11.488]</t>
+  </si>
+  <si>
+    <t>[83.417-83.5363]</t>
+  </si>
+  <si>
+    <t>[83.5363-83.6556]</t>
+  </si>
+  <si>
+    <t>[83.6556-83.7749]</t>
+  </si>
+  <si>
+    <t>[83.7749-83.8942]</t>
+  </si>
+  <si>
+    <t>[83.8942-84.0134]</t>
+  </si>
+  <si>
+    <t>[84.0134-84.1327]</t>
+  </si>
+  <si>
+    <t>[84.1327-84.252]</t>
+  </si>
+  <si>
+    <t>[84.252-84.3713]</t>
+  </si>
+  <si>
+    <t>[84.3713-84.4906]</t>
+  </si>
+  <si>
+    <t>[84.4906-84.6099]</t>
+  </si>
+  <si>
+    <t>[84.6099-84.7292]</t>
+  </si>
+  <si>
+    <t>[84.7292-84.8485]</t>
+  </si>
+  <si>
+    <t>[84.8485-84.9677]</t>
+  </si>
+  <si>
+    <t>[84.9677-85.087]</t>
+  </si>
+  <si>
+    <t>[83.6033-83.6958]</t>
+  </si>
+  <si>
+    <t>[83.6958-83.7883]</t>
+  </si>
+  <si>
+    <t>[83.7883-83.8807]</t>
+  </si>
+  <si>
+    <t>[83.8807-83.9732]</t>
+  </si>
+  <si>
+    <t>[83.9732-84.0657]</t>
+  </si>
+  <si>
+    <t>[84.0657-84.1582]</t>
+  </si>
+  <si>
+    <t>[84.1582-84.2506]</t>
+  </si>
+  <si>
+    <t>[84.2506-84.3431]</t>
+  </si>
+  <si>
+    <t>[84.3431-84.4356]</t>
+  </si>
+  <si>
+    <t>[84.4356-84.5281]</t>
+  </si>
+  <si>
+    <t>[84.5281-84.6205]</t>
+  </si>
+  <si>
+    <t>[84.6205-84.713]</t>
+  </si>
+  <si>
+    <t>[84.713-84.8055]</t>
+  </si>
+  <si>
+    <t>[84.8055-84.8979]</t>
+  </si>
+  <si>
+    <t>[83.417-83.5313]</t>
+  </si>
+  <si>
+    <t>[83.5313-83.6456]</t>
+  </si>
+  <si>
+    <t>[83.6456-83.7598]</t>
+  </si>
+  <si>
+    <t>[83.7598-83.8741]</t>
+  </si>
+  <si>
+    <t>[83.8741-83.9884]</t>
+  </si>
+  <si>
+    <t>[83.9884-84.1027]</t>
+  </si>
+  <si>
+    <t>[84.1027-84.217]</t>
+  </si>
+  <si>
+    <t>[84.217-84.3313]</t>
+  </si>
+  <si>
+    <t>[84.3313-84.4455]</t>
+  </si>
+  <si>
+    <t>[84.4455-84.5598]</t>
+  </si>
+  <si>
+    <t>[84.5598-84.6741]</t>
+  </si>
+  <si>
+    <t>[84.6741-84.7884]</t>
+  </si>
+  <si>
+    <t>[84.7884-84.9027]</t>
+  </si>
+  <si>
+    <t>[84.9027-85.0169]</t>
+  </si>
+  <si>
+    <t>[83.9234-84.0065]</t>
+  </si>
+  <si>
+    <t>[84.0065-84.0896]</t>
+  </si>
+  <si>
+    <t>[84.0896-84.1728]</t>
+  </si>
+  <si>
+    <t>[84.1728-84.2559]</t>
+  </si>
+  <si>
+    <t>[84.2559-84.339]</t>
+  </si>
+  <si>
+    <t>[84.339-84.4221]</t>
+  </si>
+  <si>
+    <t>[84.4221-84.5052]</t>
+  </si>
+  <si>
+    <t>[84.5052-84.5883]</t>
+  </si>
+  <si>
+    <t>[84.5883-84.6715]</t>
+  </si>
+  <si>
+    <t>[84.6715-84.7546]</t>
+  </si>
+  <si>
+    <t>[84.7546-84.8377]</t>
+  </si>
+  <si>
+    <t>[84.8377-84.9208]</t>
+  </si>
+  <si>
+    <t>[84.9208-85.0039]</t>
+  </si>
+  <si>
+    <t>[85.0039-85.087]</t>
   </si>
 </sst>
 </file>
@@ -694,46 +691,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>[23.0-24.0]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[24.0-24.0]</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>[24.0-25.0]</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>[25.0-25.0]</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>[25.0-26.0]</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>[26.0-26.0]</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>[26.0-27.0]</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>[27.0-28.0]</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>[28.0-28.0]</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>[28.0-29.0]</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
+                  <c:v>[29.0-29.0]</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>[29.0-30.0]</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>[30.0-30.0]</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>[30.0-31.0]</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
+                  <c:v>[31.0-31.0]</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>[31.0-32.0]</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>[32.0-33.0]</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>[33.0-33.0]</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>[33.0-34.0]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -751,34 +748,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -911,46 +908,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[10.442-10.521]</c:v>
+                  <c:v>[10.26-10.349]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[10.521-10.601]</c:v>
+                  <c:v>[10.349-10.439]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[10.601-10.681]</c:v>
+                  <c:v>[10.439-10.529]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[10.681-10.761]</c:v>
+                  <c:v>[10.529-10.619]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[10.761-10.84]</c:v>
+                  <c:v>[10.619-10.709]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[10.84-10.92]</c:v>
+                  <c:v>[10.709-10.798]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.92-11.0]</c:v>
+                  <c:v>[10.798-10.888]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[11.0-11.079]</c:v>
+                  <c:v>[10.888-10.978]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[11.079-11.159]</c:v>
+                  <c:v>[10.978-11.068]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[11.159-11.239]</c:v>
+                  <c:v>[11.068-11.157]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.239-11.319]</c:v>
+                  <c:v>[11.157-11.247]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.319-11.398]</c:v>
+                  <c:v>[11.247-11.337]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.398-11.478]</c:v>
+                  <c:v>[11.337-11.427]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.478-11.558]</c:v>
+                  <c:v>[11.427-11.517]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -965,19 +962,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -986,16 +983,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1138,46 +1135,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[9.894-9.983]</c:v>
+                  <c:v>[9.829-9.916]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[9.983-10.072]</c:v>
+                  <c:v>[9.916-10.003]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[10.072-10.162]</c:v>
+                  <c:v>[10.003-10.09]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[10.162-10.251]</c:v>
+                  <c:v>[10.09-10.177]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[10.251-10.34]</c:v>
+                  <c:v>[10.177-10.264]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[10.34-10.429]</c:v>
+                  <c:v>[10.264-10.351]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.429-10.519]</c:v>
+                  <c:v>[10.351-10.438]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.519-10.608]</c:v>
+                  <c:v>[10.438-10.526]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.608-10.697]</c:v>
+                  <c:v>[10.526-10.613]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.697-10.787]</c:v>
+                  <c:v>[10.613-10.7]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[10.787-10.876]</c:v>
+                  <c:v>[10.7-10.787]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[10.876-10.965]</c:v>
+                  <c:v>[10.787-10.874]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[10.965-11.055]</c:v>
+                  <c:v>[10.874-10.961]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.055-11.144]</c:v>
+                  <c:v>[10.961-11.048]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1192,13 +1189,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1213,19 +1210,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -1365,46 +1362,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[10.906-10.953]</c:v>
+                  <c:v>[10.65-10.71]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[10.953-11.0]</c:v>
+                  <c:v>[10.71-10.77]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[11.0-11.047]</c:v>
+                  <c:v>[10.77-10.83]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[11.047-11.094]</c:v>
+                  <c:v>[10.83-10.89]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[11.094-11.141]</c:v>
+                  <c:v>[10.89-10.949]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[11.141-11.188]</c:v>
+                  <c:v>[10.949-11.009]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[11.188-11.235]</c:v>
+                  <c:v>[11.009-11.069]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[11.235-11.282]</c:v>
+                  <c:v>[11.069-11.129]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[11.282-11.329]</c:v>
+                  <c:v>[11.129-11.189]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[11.329-11.376]</c:v>
+                  <c:v>[11.189-11.248]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.376-11.422]</c:v>
+                  <c:v>[11.248-11.308]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.422-11.469]</c:v>
+                  <c:v>[11.308-11.368]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.469-11.516]</c:v>
+                  <c:v>[11.368-11.428]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.516-11.563]</c:v>
+                  <c:v>[11.428-11.488]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1416,28 +1413,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1449,13 +1446,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1592,46 +1589,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.8352-0.8363]</c:v>
+                  <c:v>[83.417-83.5363]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.8363-0.8374]</c:v>
+                  <c:v>[83.5363-83.6556]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.8374-0.8385]</c:v>
+                  <c:v>[83.6556-83.7749]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.8385-0.8395]</c:v>
+                  <c:v>[83.7749-83.8942]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.8395-0.8406]</c:v>
+                  <c:v>[83.8942-84.0134]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.8406-0.8417]</c:v>
+                  <c:v>[84.0134-84.1327]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8417-0.8428]</c:v>
+                  <c:v>[84.1327-84.252]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.8428-0.8439]</c:v>
+                  <c:v>[84.252-84.3713]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8439-0.845]</c:v>
+                  <c:v>[84.3713-84.4906]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.845-0.8461]</c:v>
+                  <c:v>[84.4906-84.6099]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.8461-0.8472]</c:v>
+                  <c:v>[84.6099-84.7292]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.8472-0.8483]</c:v>
+                  <c:v>[84.7292-84.8485]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.8483-0.8494]</c:v>
+                  <c:v>[84.8485-84.9677]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[0.8494-0.8505]</c:v>
+                  <c:v>[84.9677-85.087]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1652,37 +1649,37 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1715,7 +1712,7 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000" vert="horz"/>
@@ -1819,46 +1816,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.8387-0.8393]</c:v>
+                  <c:v>[83.6033-83.6958]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.8393-0.8399]</c:v>
+                  <c:v>[83.6958-83.7883]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.8399-0.8406]</c:v>
+                  <c:v>[83.7883-83.8807]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.8406-0.8412]</c:v>
+                  <c:v>[83.8807-83.9732]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.8412-0.8418]</c:v>
+                  <c:v>[83.9732-84.0657]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.8418-0.8424]</c:v>
+                  <c:v>[84.0657-84.1582]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8424-0.8431]</c:v>
+                  <c:v>[84.1582-84.2506]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.8431-0.8437]</c:v>
+                  <c:v>[84.2506-84.3431]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8437-0.8443]</c:v>
+                  <c:v>[84.3431-84.4356]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.8443-0.8449]</c:v>
+                  <c:v>[84.4356-84.5281]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.8449-0.8456]</c:v>
+                  <c:v>[84.5281-84.6205]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.8456-0.8462]</c:v>
+                  <c:v>[84.6205-84.713]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.8462-0.8468]</c:v>
+                  <c:v>[84.713-84.8055]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[0.8468-0.8475]</c:v>
+                  <c:v>[84.8055-84.8979]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1870,10 +1867,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1882,7 +1879,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1891,25 +1888,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1942,7 +1939,7 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000" vert="horz"/>
@@ -2046,46 +2043,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.8352-0.8361]</c:v>
+                  <c:v>[83.417-83.5313]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.8361-0.8369]</c:v>
+                  <c:v>[83.5313-83.6456]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.8369-0.8378]</c:v>
+                  <c:v>[83.6456-83.7598]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.8378-0.8387]</c:v>
+                  <c:v>[83.7598-83.8741]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.8387-0.8396]</c:v>
+                  <c:v>[83.8741-83.9884]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.8396-0.8405]</c:v>
+                  <c:v>[83.9884-84.1027]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8405-0.8414]</c:v>
+                  <c:v>[84.1027-84.217]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.8414-0.8423]</c:v>
+                  <c:v>[84.217-84.3313]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8423-0.8432]</c:v>
+                  <c:v>[84.3313-84.4455]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.8432-0.844]</c:v>
+                  <c:v>[84.4455-84.5598]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.844-0.8449]</c:v>
+                  <c:v>[84.5598-84.6741]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.8449-0.8458]</c:v>
+                  <c:v>[84.6741-84.7884]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.8458-0.8467]</c:v>
+                  <c:v>[84.7884-84.9027]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[0.8467-0.8476]</c:v>
+                  <c:v>[84.9027-85.0169]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2103,22 +2100,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2127,16 +2124,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2169,7 +2166,7 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000" vert="horz"/>
@@ -2273,46 +2270,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[0.8366-0.8376]</c:v>
+                  <c:v>[83.9234-84.0065]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[0.8376-0.8386]</c:v>
+                  <c:v>[84.0065-84.0896]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[0.8386-0.8396]</c:v>
+                  <c:v>[84.0896-84.1728]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[0.8396-0.8406]</c:v>
+                  <c:v>[84.1728-84.2559]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[0.8406-0.8416]</c:v>
+                  <c:v>[84.2559-84.339]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[0.8416-0.8426]</c:v>
+                  <c:v>[84.339-84.4221]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[0.8426-0.8435]</c:v>
+                  <c:v>[84.4221-84.5052]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[0.8435-0.8445]</c:v>
+                  <c:v>[84.5052-84.5883]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[0.8445-0.8455]</c:v>
+                  <c:v>[84.5883-84.6715]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[0.8455-0.8465]</c:v>
+                  <c:v>[84.6715-84.7546]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[0.8465-0.8475]</c:v>
+                  <c:v>[84.7546-84.8377]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[0.8475-0.8485]</c:v>
+                  <c:v>[84.8377-84.9208]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[0.8485-0.8495]</c:v>
+                  <c:v>[84.9208-85.0039]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[0.8495-0.8505]</c:v>
+                  <c:v>[85.0039-85.087]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2336,28 +2333,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2396,7 +2393,7 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="-2700000" vert="horz"/>
@@ -2500,28 +2497,28 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>[23.0-24.0]</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>[24.0-24.0]</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>[24.0-25.0]</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>[25.0-25.0]</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>[25.0-26.0]</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>[26.0-26.0]</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>[26.0-26.0]</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>[26.0-27.0]</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>[27.0-28.0]</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>[28.0-28.0]</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>[28.0-28.0]</c:v>
@@ -2530,10 +2527,10 @@
                   <c:v>[28.0-29.0]</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>[29.0-29.0]</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>[29.0-30.0]</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>[30.0-30.0]</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>[30.0-30.0]</c:v>
@@ -2563,28 +2560,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2780,7 +2777,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2789,7 +2786,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2943,37 +2940,37 @@
                   <c:v>[25.0-26.0]</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>[26.0-26.0]</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>[26.0-27.0]</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>[27.0-27.0]</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>[27.0-28.0]</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>[28.0-28.0]</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>[28.0-29.0]</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>[29.0-29.0]</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>[29.0-30.0]</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>[30.0-30.0]</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>[30.0-31.0]</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
+                  <c:v>[31.0-31.0]</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>[31.0-32.0]</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>[32.0-33.0]</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>[33.0-33.0]</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>[33.0-34.0]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2997,13 +2994,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
@@ -3012,13 +3009,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -3151,46 +3148,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.8214-3.8416]</c:v>
+                  <c:v>[3.8313-3.8516]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.8416-3.8618]</c:v>
+                  <c:v>[3.8516-3.8718]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.8618-3.882]</c:v>
+                  <c:v>[3.8718-3.8921]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.882-3.9022]</c:v>
+                  <c:v>[3.8921-3.9123]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.9022-3.9225]</c:v>
+                  <c:v>[3.9123-3.9326]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9225-3.9427]</c:v>
+                  <c:v>[3.9326-3.9528]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.9427-3.9629]</c:v>
+                  <c:v>[3.9528-3.9731]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.9629-3.9831]</c:v>
+                  <c:v>[3.9731-3.9933]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.9831-4.0033]</c:v>
+                  <c:v>[3.9933-4.0136]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.0033-4.0235]</c:v>
+                  <c:v>[4.0136-4.0338]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.0235-4.0438]</c:v>
+                  <c:v>[4.0338-4.0541]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.0438-4.064]</c:v>
+                  <c:v>[4.0541-4.0743]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.064-4.0842]</c:v>
+                  <c:v>[4.0743-4.0946]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.0842-4.1044]</c:v>
+                  <c:v>[4.0946-4.1148]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3205,40 +3202,40 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -3267,7 +3264,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Weighted Average Cost of Fund (%)</a:t>
+                  <a:t>Weighted Average Cost of Funds (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3378,46 +3375,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.8247-3.8381]</c:v>
+                  <c:v>[3.8313-3.8464]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.8381-3.8515]</c:v>
+                  <c:v>[3.8464-3.8614]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.8515-3.865]</c:v>
+                  <c:v>[3.8614-3.8765]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.865-3.8784]</c:v>
+                  <c:v>[3.8765-3.8915]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.8784-3.8918]</c:v>
+                  <c:v>[3.8915-3.9066]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.8918-3.9052]</c:v>
+                  <c:v>[3.9066-3.9216]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.9052-3.9187]</c:v>
+                  <c:v>[3.9216-3.9367]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.9187-3.9321]</c:v>
+                  <c:v>[3.9367-3.9517]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.9321-3.9455]</c:v>
+                  <c:v>[3.9517-3.9668]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.9455-3.959]</c:v>
+                  <c:v>[3.9668-3.9818]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.959-3.9724]</c:v>
+                  <c:v>[3.9818-3.9969]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.9724-3.9858]</c:v>
+                  <c:v>[3.9969-4.0119]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.9858-3.9993]</c:v>
+                  <c:v>[4.0119-4.027]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.9993-4.0127]</c:v>
+                  <c:v>[4.027-4.042]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3435,16 +3432,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3453,7 +3450,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -3465,7 +3462,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -3494,7 +3491,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Weighted Average Cost of Fund (%)</a:t>
+                  <a:t>Weighted Average Cost of Funds (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3605,46 +3602,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.8941-3.9091]</c:v>
+                  <c:v>[3.9146-3.9289]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.9091-3.9242]</c:v>
+                  <c:v>[3.9289-3.9432]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.9242-3.9392]</c:v>
+                  <c:v>[3.9432-3.9575]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.9392-3.9542]</c:v>
+                  <c:v>[3.9575-3.9718]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.9542-3.9692]</c:v>
+                  <c:v>[3.9718-3.9861]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9692-3.9842]</c:v>
+                  <c:v>[3.9861-4.0004]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.9842-3.9993]</c:v>
+                  <c:v>[4.0004-4.0147]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.9993-4.0143]</c:v>
+                  <c:v>[4.0147-4.029]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.0143-4.0293]</c:v>
+                  <c:v>[4.029-4.0433]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.0293-4.0443]</c:v>
+                  <c:v>[4.0433-4.0576]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.0443-4.0594]</c:v>
+                  <c:v>[4.0576-4.0719]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.0594-4.0744]</c:v>
+                  <c:v>[4.0719-4.0862]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.0744-4.0894]</c:v>
+                  <c:v>[4.0862-4.1005]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.0894-4.1044]</c:v>
+                  <c:v>[4.1005-4.1148]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3659,19 +3656,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3686,13 +3683,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -3721,7 +3718,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Weighted Average Cost of Fund (%)</a:t>
+                  <a:t>Weighted Average Cost of Funds (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3832,46 +3829,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.8214-3.8297]</c:v>
+                  <c:v>[3.8347-3.8449]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.8297-3.838]</c:v>
+                  <c:v>[3.8449-3.8551]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.838-3.8463]</c:v>
+                  <c:v>[3.8551-3.8653]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.8463-3.8547]</c:v>
+                  <c:v>[3.8653-3.8755]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.8547-3.863]</c:v>
+                  <c:v>[3.8755-3.8857]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.863-3.8713]</c:v>
+                  <c:v>[3.8857-3.8959]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.8713-3.8796]</c:v>
+                  <c:v>[3.8959-3.9061]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.8796-3.8879]</c:v>
+                  <c:v>[3.9061-3.9163]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.8879-3.8962]</c:v>
+                  <c:v>[3.9163-3.9265]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.8962-3.9046]</c:v>
+                  <c:v>[3.9265-3.9367]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.9046-3.9129]</c:v>
+                  <c:v>[3.9367-3.9469]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.9129-3.9212]</c:v>
+                  <c:v>[3.9469-3.9571]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.9212-3.9295]</c:v>
+                  <c:v>[3.9571-3.9673]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.9295-3.9378]</c:v>
+                  <c:v>[3.9673-3.9775]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3883,31 +3880,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -3919,10 +3916,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3948,7 +3945,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Weighted Average Cost of Fund (%)</a:t>
+                  <a:t>Weighted Average Cost of Funds (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4059,46 +4056,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[9.894-10.013]</c:v>
+                  <c:v>[9.829-9.95]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[10.013-10.132]</c:v>
+                  <c:v>[9.95-10.07]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[10.132-10.251]</c:v>
+                  <c:v>[10.07-10.191]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[10.251-10.371]</c:v>
+                  <c:v>[10.191-10.311]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[10.371-10.49]</c:v>
+                  <c:v>[10.311-10.432]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[10.49-10.609]</c:v>
+                  <c:v>[10.432-10.552]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.609-10.728]</c:v>
+                  <c:v>[10.552-10.673]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.728-10.848]</c:v>
+                  <c:v>[10.673-10.793]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.848-10.967]</c:v>
+                  <c:v>[10.793-10.914]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.967-11.086]</c:v>
+                  <c:v>[10.914-11.034]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.086-11.205]</c:v>
+                  <c:v>[11.034-11.155]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.205-11.325]</c:v>
+                  <c:v>[11.155-11.276]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.325-11.444]</c:v>
+                  <c:v>[11.276-11.396]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.444-11.563]</c:v>
+                  <c:v>[11.396-11.517]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4113,40 +4110,40 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2</c:v>
@@ -5118,7 +5115,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5126,7 +5123,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5134,7 +5131,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5142,7 +5139,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5150,7 +5147,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5158,7 +5155,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5166,7 +5163,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5174,7 +5171,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5182,7 +5179,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5190,7 +5187,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5225,7 +5222,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5233,23 +5230,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5257,23 +5254,23 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5281,7 +5278,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5289,23 +5286,23 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -5313,15 +5310,15 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5329,7 +5326,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5351,7 +5348,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5359,15 +5356,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5375,15 +5372,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5391,7 +5388,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5399,7 +5396,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5407,7 +5404,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5415,47 +5412,47 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5477,39 +5474,39 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5517,31 +5514,31 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -5549,7 +5546,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -5557,7 +5554,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5565,15 +5562,15 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5581,10 +5578,10 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5603,7 +5600,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5611,7 +5608,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5619,7 +5616,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5627,15 +5624,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -5643,15 +5640,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5659,58 +5656,58 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5729,23 +5726,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5753,7 +5750,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5761,15 +5758,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5777,7 +5774,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5785,15 +5782,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -5801,23 +5798,23 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5825,18 +5822,18 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5855,7 +5852,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5863,7 +5860,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5871,39 +5868,39 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5911,15 +5908,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -5927,7 +5924,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5935,23 +5932,23 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5959,10 +5956,10 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5981,7 +5978,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -5989,7 +5986,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5997,7 +5994,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6005,7 +6002,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -6013,15 +6010,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6029,23 +6026,23 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -6053,31 +6050,31 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6085,7 +6082,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6107,7 +6104,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6115,7 +6112,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6131,7 +6128,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -6139,15 +6136,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6155,23 +6152,23 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6179,15 +6176,15 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6195,15 +6192,15 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6211,7 +6208,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6233,7 +6230,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6241,7 +6238,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6249,7 +6246,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6257,7 +6254,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -6265,15 +6262,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6281,7 +6278,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -6289,10 +6286,10 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6305,7 +6302,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6313,7 +6310,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6321,7 +6318,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6329,7 +6326,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -6337,7 +6334,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -6359,7 +6356,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6367,7 +6364,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6375,7 +6372,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6383,7 +6380,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -6391,15 +6388,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6410,12 +6407,12 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -6423,7 +6420,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -6431,15 +6428,15 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6450,7 +6447,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6485,7 +6482,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1">
         <v>2</v>
@@ -6493,71 +6490,71 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6565,31 +6562,31 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6611,7 +6608,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -6619,7 +6616,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6627,39 +6624,39 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6667,7 +6664,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6675,15 +6672,15 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6691,7 +6688,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -6699,7 +6696,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6707,15 +6704,15 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6737,7 +6734,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -6745,47 +6742,47 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6793,7 +6790,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -6801,7 +6798,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6809,7 +6806,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6817,15 +6814,15 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -6833,15 +6830,15 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6863,79 +6860,79 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -6943,7 +6940,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -6951,7 +6948,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6959,18 +6956,18 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6989,7 +6986,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -6997,55 +6994,55 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -7053,47 +7050,47 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>2</v>

</xml_diff>

<commit_message>
added all_tranches list in clo class
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -29,507 +29,504 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="167">
-  <si>
-    <t>[3.7924-3.8222]</t>
-  </si>
-  <si>
-    <t>[3.8222-3.852]</t>
-  </si>
-  <si>
-    <t>[3.852-3.8817]</t>
-  </si>
-  <si>
-    <t>[3.8817-3.9115]</t>
-  </si>
-  <si>
-    <t>[3.9115-3.9413]</t>
-  </si>
-  <si>
-    <t>[3.9413-3.971]</t>
-  </si>
-  <si>
-    <t>[3.971-4.0008]</t>
-  </si>
-  <si>
-    <t>[4.0008-4.0306]</t>
-  </si>
-  <si>
-    <t>[4.0306-4.0603]</t>
-  </si>
-  <si>
-    <t>[4.0603-4.0901]</t>
-  </si>
-  <si>
-    <t>[4.0901-4.1199]</t>
-  </si>
-  <si>
-    <t>[4.1199-4.1496]</t>
-  </si>
-  <si>
-    <t>[4.1496-4.1794]</t>
-  </si>
-  <si>
-    <t>[4.1794-4.2092]</t>
-  </si>
-  <si>
-    <t>[3.8259-3.8431]</t>
-  </si>
-  <si>
-    <t>[3.8431-3.8603]</t>
-  </si>
-  <si>
-    <t>[3.8603-3.8776]</t>
-  </si>
-  <si>
-    <t>[3.8776-3.8948]</t>
-  </si>
-  <si>
-    <t>[3.8948-3.912]</t>
-  </si>
-  <si>
-    <t>[3.912-3.9292]</t>
-  </si>
-  <si>
-    <t>[3.9292-3.9464]</t>
-  </si>
-  <si>
-    <t>[3.9464-3.9637]</t>
-  </si>
-  <si>
-    <t>[3.9637-3.9809]</t>
-  </si>
-  <si>
-    <t>[3.9809-3.9981]</t>
-  </si>
-  <si>
-    <t>[3.9981-4.0153]</t>
-  </si>
-  <si>
-    <t>[4.0153-4.0325]</t>
-  </si>
-  <si>
-    <t>[4.0325-4.0497]</t>
-  </si>
-  <si>
-    <t>[4.0497-4.067]</t>
-  </si>
-  <si>
-    <t>[3.8687-3.893]</t>
-  </si>
-  <si>
-    <t>[3.893-3.9173]</t>
-  </si>
-  <si>
-    <t>[3.9173-3.9416]</t>
-  </si>
-  <si>
-    <t>[3.9416-3.966]</t>
-  </si>
-  <si>
-    <t>[3.966-3.9903]</t>
-  </si>
-  <si>
-    <t>[3.9903-4.0146]</t>
-  </si>
-  <si>
-    <t>[4.0146-4.0389]</t>
-  </si>
-  <si>
-    <t>[4.0389-4.0633]</t>
-  </si>
-  <si>
-    <t>[4.0633-4.0876]</t>
-  </si>
-  <si>
-    <t>[4.0876-4.1119]</t>
-  </si>
-  <si>
-    <t>[4.1119-4.1362]</t>
-  </si>
-  <si>
-    <t>[4.1362-4.1605]</t>
-  </si>
-  <si>
-    <t>[4.1605-4.1849]</t>
-  </si>
-  <si>
-    <t>[4.1849-4.2092]</t>
-  </si>
-  <si>
-    <t>[3.7924-3.8103]</t>
-  </si>
-  <si>
-    <t>[3.8103-3.8281]</t>
-  </si>
-  <si>
-    <t>[3.8281-3.846]</t>
-  </si>
-  <si>
-    <t>[3.846-3.8639]</t>
-  </si>
-  <si>
-    <t>[3.8639-3.8817]</t>
-  </si>
-  <si>
-    <t>[3.8817-3.8996]</t>
-  </si>
-  <si>
-    <t>[3.8996-3.9175]</t>
-  </si>
-  <si>
-    <t>[3.9175-3.9353]</t>
-  </si>
-  <si>
-    <t>[3.9353-3.9532]</t>
-  </si>
-  <si>
-    <t>[3.9532-3.9711]</t>
-  </si>
-  <si>
-    <t>[3.9711-3.9889]</t>
-  </si>
-  <si>
-    <t>[3.9889-4.0068]</t>
-  </si>
-  <si>
-    <t>[4.0068-4.0247]</t>
-  </si>
-  <si>
-    <t>[4.0247-4.0425]</t>
-  </si>
-  <si>
-    <t>[9.255-9.434]</t>
-  </si>
-  <si>
-    <t>[9.434-9.613]</t>
-  </si>
-  <si>
-    <t>[9.613-9.792]</t>
-  </si>
-  <si>
-    <t>[9.792-9.97]</t>
-  </si>
-  <si>
-    <t>[9.97-10.149]</t>
-  </si>
-  <si>
-    <t>[10.149-10.328]</t>
-  </si>
-  <si>
-    <t>[10.328-10.507]</t>
-  </si>
-  <si>
-    <t>[10.507-10.685]</t>
-  </si>
-  <si>
-    <t>[10.685-10.864]</t>
-  </si>
-  <si>
-    <t>[10.864-11.043]</t>
-  </si>
-  <si>
-    <t>[11.043-11.222]</t>
-  </si>
-  <si>
-    <t>[11.222-11.4]</t>
-  </si>
-  <si>
-    <t>[11.4-11.579]</t>
-  </si>
-  <si>
-    <t>[11.579-11.758]</t>
-  </si>
-  <si>
-    <t>[10.105-10.208]</t>
-  </si>
-  <si>
-    <t>[10.208-10.311]</t>
-  </si>
-  <si>
-    <t>[10.311-10.414]</t>
-  </si>
-  <si>
-    <t>[10.414-10.518]</t>
-  </si>
-  <si>
-    <t>[10.518-10.621]</t>
-  </si>
-  <si>
-    <t>[10.621-10.724]</t>
-  </si>
-  <si>
-    <t>[10.724-10.827]</t>
-  </si>
-  <si>
-    <t>[10.827-10.931]</t>
-  </si>
-  <si>
-    <t>[10.931-11.034]</t>
-  </si>
-  <si>
-    <t>[11.034-11.137]</t>
-  </si>
-  <si>
-    <t>[11.137-11.24]</t>
-  </si>
-  <si>
-    <t>[11.24-11.344]</t>
-  </si>
-  <si>
-    <t>[11.344-11.447]</t>
-  </si>
-  <si>
-    <t>[11.447-11.55]</t>
-  </si>
-  <si>
-    <t>[9.255-9.402]</t>
-  </si>
-  <si>
-    <t>[9.402-9.549]</t>
-  </si>
-  <si>
-    <t>[9.549-9.696]</t>
-  </si>
-  <si>
-    <t>[9.696-9.843]</t>
-  </si>
-  <si>
-    <t>[9.843-9.99]</t>
-  </si>
-  <si>
-    <t>[9.99-10.136]</t>
-  </si>
-  <si>
-    <t>[10.136-10.283]</t>
-  </si>
-  <si>
-    <t>[10.283-10.43]</t>
-  </si>
-  <si>
-    <t>[10.43-10.577]</t>
-  </si>
-  <si>
-    <t>[10.577-10.724]</t>
-  </si>
-  <si>
-    <t>[10.724-10.871]</t>
-  </si>
-  <si>
-    <t>[10.871-11.018]</t>
-  </si>
-  <si>
-    <t>[11.018-11.164]</t>
-  </si>
-  <si>
-    <t>[11.164-11.311]</t>
-  </si>
-  <si>
-    <t>[10.278-10.383]</t>
-  </si>
-  <si>
-    <t>[10.383-10.489]</t>
-  </si>
-  <si>
-    <t>[10.489-10.595]</t>
-  </si>
-  <si>
-    <t>[10.595-10.701]</t>
-  </si>
-  <si>
-    <t>[10.701-10.806]</t>
-  </si>
-  <si>
-    <t>[10.806-10.912]</t>
-  </si>
-  <si>
-    <t>[10.912-11.018]</t>
-  </si>
-  <si>
-    <t>[11.018-11.124]</t>
-  </si>
-  <si>
-    <t>[11.124-11.229]</t>
-  </si>
-  <si>
-    <t>[11.229-11.335]</t>
-  </si>
-  <si>
-    <t>[11.335-11.441]</t>
-  </si>
-  <si>
-    <t>[11.441-11.547]</t>
-  </si>
-  <si>
-    <t>[11.547-11.652]</t>
-  </si>
-  <si>
-    <t>[11.652-11.758]</t>
-  </si>
-  <si>
-    <t>[82.94-83.1]</t>
-  </si>
-  <si>
-    <t>[83.1-83.27]</t>
-  </si>
-  <si>
-    <t>[83.27-83.44]</t>
-  </si>
-  <si>
-    <t>[83.44-83.61]</t>
-  </si>
-  <si>
-    <t>[83.61-83.78]</t>
-  </si>
-  <si>
-    <t>[83.78-83.95]</t>
-  </si>
-  <si>
-    <t>[83.95-84.11]</t>
-  </si>
-  <si>
-    <t>[84.11-84.28]</t>
-  </si>
-  <si>
-    <t>[84.28-84.45]</t>
-  </si>
-  <si>
-    <t>[84.45-84.62]</t>
-  </si>
-  <si>
-    <t>[84.62-84.79]</t>
-  </si>
-  <si>
-    <t>[84.79-84.96]</t>
-  </si>
-  <si>
-    <t>[84.96-85.12]</t>
-  </si>
-  <si>
-    <t>[85.12-85.29]</t>
-  </si>
-  <si>
-    <t>[83.41-83.55]</t>
-  </si>
-  <si>
-    <t>[83.55-83.68]</t>
-  </si>
-  <si>
-    <t>[83.68-83.82]</t>
-  </si>
-  <si>
-    <t>[83.82-83.95]</t>
-  </si>
-  <si>
-    <t>[83.95-84.08]</t>
-  </si>
-  <si>
-    <t>[84.08-84.22]</t>
-  </si>
-  <si>
-    <t>[84.22-84.35]</t>
-  </si>
-  <si>
-    <t>[84.35-84.49]</t>
-  </si>
-  <si>
-    <t>[84.49-84.62]</t>
-  </si>
-  <si>
-    <t>[84.62-84.76]</t>
-  </si>
-  <si>
-    <t>[84.76-84.89]</t>
-  </si>
-  <si>
-    <t>[84.89-85.02]</t>
-  </si>
-  <si>
-    <t>[85.02-85.16]</t>
-  </si>
-  <si>
-    <t>[85.16-85.29]</t>
-  </si>
-  <si>
-    <t>[83.1-83.26]</t>
-  </si>
-  <si>
-    <t>[83.26-83.42]</t>
-  </si>
-  <si>
-    <t>[83.42-83.58]</t>
-  </si>
-  <si>
-    <t>[83.58-83.74]</t>
-  </si>
-  <si>
-    <t>[83.74-83.9]</t>
-  </si>
-  <si>
-    <t>[83.9-84.06]</t>
-  </si>
-  <si>
-    <t>[84.06-84.22]</t>
-  </si>
-  <si>
-    <t>[84.22-84.38]</t>
-  </si>
-  <si>
-    <t>[84.38-84.54]</t>
-  </si>
-  <si>
-    <t>[84.54-84.7]</t>
-  </si>
-  <si>
-    <t>[84.7-84.86]</t>
-  </si>
-  <si>
-    <t>[84.86-85.03]</t>
-  </si>
-  <si>
-    <t>[85.03-85.19]</t>
-  </si>
-  <si>
-    <t>[83.67-83.78]</t>
-  </si>
-  <si>
-    <t>[83.78-83.89]</t>
-  </si>
-  <si>
-    <t>[83.89-84.0]</t>
-  </si>
-  <si>
-    <t>[84.0-84.11]</t>
-  </si>
-  <si>
-    <t>[84.11-84.22]</t>
-  </si>
-  <si>
-    <t>[84.22-84.33]</t>
-  </si>
-  <si>
-    <t>[84.33-84.44]</t>
-  </si>
-  <si>
-    <t>[84.44-84.55]</t>
-  </si>
-  <si>
-    <t>[84.55-84.66]</t>
-  </si>
-  <si>
-    <t>[84.66-84.77]</t>
-  </si>
-  <si>
-    <t>[84.77-84.88]</t>
-  </si>
-  <si>
-    <t>[84.88-84.99]</t>
-  </si>
-  <si>
-    <t>[84.99-85.1]</t>
-  </si>
-  <si>
-    <t>[85.1-85.21]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="166">
+  <si>
+    <t>[3.345-3.362]</t>
+  </si>
+  <si>
+    <t>[3.362-3.38]</t>
+  </si>
+  <si>
+    <t>[3.38-3.397]</t>
+  </si>
+  <si>
+    <t>[3.397-3.414]</t>
+  </si>
+  <si>
+    <t>[3.414-3.432]</t>
+  </si>
+  <si>
+    <t>[3.432-3.449]</t>
+  </si>
+  <si>
+    <t>[3.449-3.467]</t>
+  </si>
+  <si>
+    <t>[3.467-3.484]</t>
+  </si>
+  <si>
+    <t>[3.484-3.501]</t>
+  </si>
+  <si>
+    <t>[3.501-3.519]</t>
+  </si>
+  <si>
+    <t>[3.519-3.536]</t>
+  </si>
+  <si>
+    <t>[3.536-3.554]</t>
+  </si>
+  <si>
+    <t>[3.554-3.571]</t>
+  </si>
+  <si>
+    <t>[3.571-3.588]</t>
+  </si>
+  <si>
+    <t>[3.345-3.356]</t>
+  </si>
+  <si>
+    <t>[3.356-3.366]</t>
+  </si>
+  <si>
+    <t>[3.366-3.377]</t>
+  </si>
+  <si>
+    <t>[3.377-3.388]</t>
+  </si>
+  <si>
+    <t>[3.388-3.398]</t>
+  </si>
+  <si>
+    <t>[3.398-3.409]</t>
+  </si>
+  <si>
+    <t>[3.409-3.42]</t>
+  </si>
+  <si>
+    <t>[3.42-3.43]</t>
+  </si>
+  <si>
+    <t>[3.43-3.441]</t>
+  </si>
+  <si>
+    <t>[3.441-3.452]</t>
+  </si>
+  <si>
+    <t>[3.452-3.463]</t>
+  </si>
+  <si>
+    <t>[3.463-3.473]</t>
+  </si>
+  <si>
+    <t>[3.473-3.484]</t>
+  </si>
+  <si>
+    <t>[3.484-3.495]</t>
+  </si>
+  <si>
+    <t>[3.453-3.462]</t>
+  </si>
+  <si>
+    <t>[3.462-3.472]</t>
+  </si>
+  <si>
+    <t>[3.472-3.482]</t>
+  </si>
+  <si>
+    <t>[3.482-3.492]</t>
+  </si>
+  <si>
+    <t>[3.492-3.501]</t>
+  </si>
+  <si>
+    <t>[3.501-3.511]</t>
+  </si>
+  <si>
+    <t>[3.511-3.521]</t>
+  </si>
+  <si>
+    <t>[3.521-3.53]</t>
+  </si>
+  <si>
+    <t>[3.53-3.54]</t>
+  </si>
+  <si>
+    <t>[3.54-3.55]</t>
+  </si>
+  <si>
+    <t>[3.55-3.559]</t>
+  </si>
+  <si>
+    <t>[3.559-3.569]</t>
+  </si>
+  <si>
+    <t>[3.569-3.579]</t>
+  </si>
+  <si>
+    <t>[3.579-3.588]</t>
+  </si>
+  <si>
+    <t>[3.353-3.365]</t>
+  </si>
+  <si>
+    <t>[3.365-3.378]</t>
+  </si>
+  <si>
+    <t>[3.378-3.39]</t>
+  </si>
+  <si>
+    <t>[3.39-3.402]</t>
+  </si>
+  <si>
+    <t>[3.402-3.415]</t>
+  </si>
+  <si>
+    <t>[3.415-3.427]</t>
+  </si>
+  <si>
+    <t>[3.427-3.439]</t>
+  </si>
+  <si>
+    <t>[3.439-3.451]</t>
+  </si>
+  <si>
+    <t>[3.451-3.464]</t>
+  </si>
+  <si>
+    <t>[3.464-3.476]</t>
+  </si>
+  <si>
+    <t>[3.476-3.488]</t>
+  </si>
+  <si>
+    <t>[3.488-3.501]</t>
+  </si>
+  <si>
+    <t>[3.501-3.513]</t>
+  </si>
+  <si>
+    <t>[3.513-3.525]</t>
+  </si>
+  <si>
+    <t>[11.46-11.53]</t>
+  </si>
+  <si>
+    <t>[11.53-11.6]</t>
+  </si>
+  <si>
+    <t>[11.6-11.67]</t>
+  </si>
+  <si>
+    <t>[11.67-11.74]</t>
+  </si>
+  <si>
+    <t>[11.74-11.81]</t>
+  </si>
+  <si>
+    <t>[11.81-11.87]</t>
+  </si>
+  <si>
+    <t>[11.87-11.94]</t>
+  </si>
+  <si>
+    <t>[11.94-12.01]</t>
+  </si>
+  <si>
+    <t>[12.01-12.08]</t>
+  </si>
+  <si>
+    <t>[12.08-12.15]</t>
+  </si>
+  <si>
+    <t>[12.15-12.22]</t>
+  </si>
+  <si>
+    <t>[12.22-12.29]</t>
+  </si>
+  <si>
+    <t>[12.29-12.35]</t>
+  </si>
+  <si>
+    <t>[12.35-12.42]</t>
+  </si>
+  <si>
+    <t>[11.82-11.86]</t>
+  </si>
+  <si>
+    <t>[11.86-11.91]</t>
+  </si>
+  <si>
+    <t>[11.91-11.95]</t>
+  </si>
+  <si>
+    <t>[11.95-11.99]</t>
+  </si>
+  <si>
+    <t>[11.99-12.03]</t>
+  </si>
+  <si>
+    <t>[12.03-12.08]</t>
+  </si>
+  <si>
+    <t>[12.08-12.12]</t>
+  </si>
+  <si>
+    <t>[12.12-12.16]</t>
+  </si>
+  <si>
+    <t>[12.16-12.21]</t>
+  </si>
+  <si>
+    <t>[12.21-12.25]</t>
+  </si>
+  <si>
+    <t>[12.25-12.29]</t>
+  </si>
+  <si>
+    <t>[12.29-12.34]</t>
+  </si>
+  <si>
+    <t>[12.34-12.38]</t>
+  </si>
+  <si>
+    <t>[12.38-12.42]</t>
+  </si>
+  <si>
+    <t>[11.46-11.5]</t>
+  </si>
+  <si>
+    <t>[11.5-11.54]</t>
+  </si>
+  <si>
+    <t>[11.54-11.58]</t>
+  </si>
+  <si>
+    <t>[11.58-11.62]</t>
+  </si>
+  <si>
+    <t>[11.62-11.66]</t>
+  </si>
+  <si>
+    <t>[11.66-11.7]</t>
+  </si>
+  <si>
+    <t>[11.7-11.74]</t>
+  </si>
+  <si>
+    <t>[11.74-11.78]</t>
+  </si>
+  <si>
+    <t>[11.78-11.82]</t>
+  </si>
+  <si>
+    <t>[11.82-11.85]</t>
+  </si>
+  <si>
+    <t>[11.85-11.89]</t>
+  </si>
+  <si>
+    <t>[11.89-11.93]</t>
+  </si>
+  <si>
+    <t>[11.93-11.97]</t>
+  </si>
+  <si>
+    <t>[11.97-12.01]</t>
+  </si>
+  <si>
+    <t>[11.7-11.75]</t>
+  </si>
+  <si>
+    <t>[11.75-11.8]</t>
+  </si>
+  <si>
+    <t>[11.8-11.85]</t>
+  </si>
+  <si>
+    <t>[11.89-11.94]</t>
+  </si>
+  <si>
+    <t>[11.94-11.99]</t>
+  </si>
+  <si>
+    <t>[11.99-12.04]</t>
+  </si>
+  <si>
+    <t>[12.04-12.09]</t>
+  </si>
+  <si>
+    <t>[12.09-12.14]</t>
+  </si>
+  <si>
+    <t>[12.14-12.19]</t>
+  </si>
+  <si>
+    <t>[12.19-12.24]</t>
+  </si>
+  <si>
+    <t>[12.24-12.29]</t>
+  </si>
+  <si>
+    <t>[12.34-12.39]</t>
+  </si>
+  <si>
+    <t>[75.11-75.33]</t>
+  </si>
+  <si>
+    <t>[75.33-75.54]</t>
+  </si>
+  <si>
+    <t>[75.54-75.76]</t>
+  </si>
+  <si>
+    <t>[75.76-75.97]</t>
+  </si>
+  <si>
+    <t>[75.97-76.18]</t>
+  </si>
+  <si>
+    <t>[76.18-76.4]</t>
+  </si>
+  <si>
+    <t>[76.4-76.61]</t>
+  </si>
+  <si>
+    <t>[76.61-76.83]</t>
+  </si>
+  <si>
+    <t>[76.83-77.04]</t>
+  </si>
+  <si>
+    <t>[77.04-77.26]</t>
+  </si>
+  <si>
+    <t>[77.26-77.47]</t>
+  </si>
+  <si>
+    <t>[77.47-77.69]</t>
+  </si>
+  <si>
+    <t>[77.69-77.9]</t>
+  </si>
+  <si>
+    <t>[77.9-78.11]</t>
+  </si>
+  <si>
+    <t>[76.25-76.39]</t>
+  </si>
+  <si>
+    <t>[76.39-76.52]</t>
+  </si>
+  <si>
+    <t>[76.52-76.65]</t>
+  </si>
+  <si>
+    <t>[76.65-76.79]</t>
+  </si>
+  <si>
+    <t>[76.79-76.92]</t>
+  </si>
+  <si>
+    <t>[76.92-77.05]</t>
+  </si>
+  <si>
+    <t>[77.05-77.18]</t>
+  </si>
+  <si>
+    <t>[77.18-77.32]</t>
+  </si>
+  <si>
+    <t>[77.32-77.45]</t>
+  </si>
+  <si>
+    <t>[77.45-77.58]</t>
+  </si>
+  <si>
+    <t>[77.58-77.72]</t>
+  </si>
+  <si>
+    <t>[77.72-77.85]</t>
+  </si>
+  <si>
+    <t>[77.85-77.98]</t>
+  </si>
+  <si>
+    <t>[77.98-78.11]</t>
+  </si>
+  <si>
+    <t>[75.11-75.29]</t>
+  </si>
+  <si>
+    <t>[75.29-75.47]</t>
+  </si>
+  <si>
+    <t>[75.47-75.65]</t>
+  </si>
+  <si>
+    <t>[75.65-75.83]</t>
+  </si>
+  <si>
+    <t>[75.83-76.01]</t>
+  </si>
+  <si>
+    <t>[76.01-76.19]</t>
+  </si>
+  <si>
+    <t>[76.19-76.37]</t>
+  </si>
+  <si>
+    <t>[76.37-76.55]</t>
+  </si>
+  <si>
+    <t>[76.55-76.73]</t>
+  </si>
+  <si>
+    <t>[76.73-76.91]</t>
+  </si>
+  <si>
+    <t>[76.91-77.08]</t>
+  </si>
+  <si>
+    <t>[77.08-77.26]</t>
+  </si>
+  <si>
+    <t>[77.26-77.44]</t>
+  </si>
+  <si>
+    <t>[77.44-77.62]</t>
+  </si>
+  <si>
+    <t>[76.21-76.34]</t>
+  </si>
+  <si>
+    <t>[76.34-76.47]</t>
+  </si>
+  <si>
+    <t>[76.47-76.6]</t>
+  </si>
+  <si>
+    <t>[76.6-76.73]</t>
+  </si>
+  <si>
+    <t>[76.73-76.86]</t>
+  </si>
+  <si>
+    <t>[76.86-76.99]</t>
+  </si>
+  <si>
+    <t>[76.99-77.11]</t>
+  </si>
+  <si>
+    <t>[77.11-77.24]</t>
+  </si>
+  <si>
+    <t>[77.24-77.37]</t>
+  </si>
+  <si>
+    <t>[77.37-77.5]</t>
+  </si>
+  <si>
+    <t>[77.5-77.63]</t>
+  </si>
+  <si>
+    <t>[77.63-77.76]</t>
+  </si>
+  <si>
+    <t>[77.76-77.89]</t>
+  </si>
+  <si>
+    <t>[77.89-78.02]</t>
   </si>
 </sst>
 </file>
@@ -635,31 +632,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -674,28 +671,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -822,46 +819,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[10.105-10.208]</c:v>
+                  <c:v>[11.82-11.86]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[10.208-10.311]</c:v>
+                  <c:v>[11.86-11.91]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[10.311-10.414]</c:v>
+                  <c:v>[11.91-11.95]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[10.414-10.518]</c:v>
+                  <c:v>[11.95-11.99]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[10.518-10.621]</c:v>
+                  <c:v>[11.99-12.03]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[10.621-10.724]</c:v>
+                  <c:v>[12.03-12.08]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.724-10.827]</c:v>
+                  <c:v>[12.08-12.12]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.827-10.931]</c:v>
+                  <c:v>[12.12-12.16]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.931-11.034]</c:v>
+                  <c:v>[12.16-12.21]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[11.034-11.137]</c:v>
+                  <c:v>[12.21-12.25]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.137-11.24]</c:v>
+                  <c:v>[12.25-12.29]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.24-11.344]</c:v>
+                  <c:v>[12.29-12.34]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.344-11.447]</c:v>
+                  <c:v>[12.34-12.38]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.447-11.55]</c:v>
+                  <c:v>[12.38-12.42]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -873,46 +870,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1049,46 +1046,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[9.255-9.402]</c:v>
+                  <c:v>[11.46-11.5]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[9.402-9.549]</c:v>
+                  <c:v>[11.5-11.54]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[9.549-9.696]</c:v>
+                  <c:v>[11.54-11.58]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[9.696-9.843]</c:v>
+                  <c:v>[11.58-11.62]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[9.843-9.99]</c:v>
+                  <c:v>[11.62-11.66]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[9.99-10.136]</c:v>
+                  <c:v>[11.66-11.7]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.136-10.283]</c:v>
+                  <c:v>[11.7-11.74]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.283-10.43]</c:v>
+                  <c:v>[11.74-11.78]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.43-10.577]</c:v>
+                  <c:v>[11.78-11.82]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.577-10.724]</c:v>
+                  <c:v>[11.82-11.85]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[10.724-10.871]</c:v>
+                  <c:v>[11.85-11.89]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[10.871-11.018]</c:v>
+                  <c:v>[11.89-11.93]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.018-11.164]</c:v>
+                  <c:v>[11.93-11.97]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.164-11.311]</c:v>
+                  <c:v>[11.97-12.01]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1100,46 +1097,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1276,46 +1273,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[10.278-10.383]</c:v>
+                  <c:v>[11.7-11.75]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[10.383-10.489]</c:v>
+                  <c:v>[11.75-11.8]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[10.489-10.595]</c:v>
+                  <c:v>[11.8-11.85]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[10.595-10.701]</c:v>
+                  <c:v>[11.85-11.89]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[10.701-10.806]</c:v>
+                  <c:v>[11.89-11.94]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[10.806-10.912]</c:v>
+                  <c:v>[11.94-11.99]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.912-11.018]</c:v>
+                  <c:v>[11.99-12.04]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[11.018-11.124]</c:v>
+                  <c:v>[12.04-12.09]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[11.124-11.229]</c:v>
+                  <c:v>[12.09-12.14]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[11.229-11.335]</c:v>
+                  <c:v>[12.14-12.19]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.335-11.441]</c:v>
+                  <c:v>[12.19-12.24]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.441-11.547]</c:v>
+                  <c:v>[12.24-12.29]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.547-11.652]</c:v>
+                  <c:v>[12.29-12.34]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.652-11.758]</c:v>
+                  <c:v>[12.34-12.39]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1333,40 +1330,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1503,46 +1500,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[82.94-83.1]</c:v>
+                  <c:v>[75.11-75.33]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.1-83.27]</c:v>
+                  <c:v>[75.33-75.54]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.27-83.44]</c:v>
+                  <c:v>[75.54-75.76]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[83.44-83.61]</c:v>
+                  <c:v>[75.76-75.97]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[83.61-83.78]</c:v>
+                  <c:v>[75.97-76.18]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[83.78-83.95]</c:v>
+                  <c:v>[76.18-76.4]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[83.95-84.11]</c:v>
+                  <c:v>[76.4-76.61]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.11-84.28]</c:v>
+                  <c:v>[76.61-76.83]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.28-84.45]</c:v>
+                  <c:v>[76.83-77.04]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.45-84.62]</c:v>
+                  <c:v>[77.04-77.26]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.62-84.79]</c:v>
+                  <c:v>[77.26-77.47]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.79-84.96]</c:v>
+                  <c:v>[77.47-77.69]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[84.96-85.12]</c:v>
+                  <c:v>[77.69-77.9]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[85.12-85.29]</c:v>
+                  <c:v>[77.9-78.11]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1554,46 +1551,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>57</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>37</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1730,46 +1727,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[83.41-83.55]</c:v>
+                  <c:v>[76.25-76.39]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.55-83.68]</c:v>
+                  <c:v>[76.39-76.52]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.68-83.82]</c:v>
+                  <c:v>[76.52-76.65]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[83.82-83.95]</c:v>
+                  <c:v>[76.65-76.79]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[83.95-84.08]</c:v>
+                  <c:v>[76.79-76.92]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[84.08-84.22]</c:v>
+                  <c:v>[76.92-77.05]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[84.22-84.35]</c:v>
+                  <c:v>[77.05-77.18]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.35-84.49]</c:v>
+                  <c:v>[77.18-77.32]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.49-84.62]</c:v>
+                  <c:v>[77.32-77.45]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.62-84.76]</c:v>
+                  <c:v>[77.45-77.58]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.76-84.89]</c:v>
+                  <c:v>[77.58-77.72]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.89-85.02]</c:v>
+                  <c:v>[77.72-77.85]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[85.02-85.16]</c:v>
+                  <c:v>[77.85-77.98]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[85.16-85.29]</c:v>
+                  <c:v>[77.98-78.11]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1781,46 +1778,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1957,46 +1954,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[82.94-83.1]</c:v>
+                  <c:v>[75.11-75.29]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.1-83.26]</c:v>
+                  <c:v>[75.29-75.47]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.26-83.42]</c:v>
+                  <c:v>[75.47-75.65]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[83.42-83.58]</c:v>
+                  <c:v>[75.65-75.83]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[83.58-83.74]</c:v>
+                  <c:v>[75.83-76.01]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[83.74-83.9]</c:v>
+                  <c:v>[76.01-76.19]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[83.9-84.06]</c:v>
+                  <c:v>[76.19-76.37]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.06-84.22]</c:v>
+                  <c:v>[76.37-76.55]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.22-84.38]</c:v>
+                  <c:v>[76.55-76.73]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.38-84.54]</c:v>
+                  <c:v>[76.73-76.91]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.54-84.7]</c:v>
+                  <c:v>[76.91-77.08]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.7-84.86]</c:v>
+                  <c:v>[77.08-77.26]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[84.86-85.03]</c:v>
+                  <c:v>[77.26-77.44]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[85.03-85.19]</c:v>
+                  <c:v>[77.44-77.62]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2008,46 +2005,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2184,46 +2181,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[83.67-83.78]</c:v>
+                  <c:v>[76.21-76.34]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.78-83.89]</c:v>
+                  <c:v>[76.34-76.47]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.89-84.0]</c:v>
+                  <c:v>[76.47-76.6]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[84.0-84.11]</c:v>
+                  <c:v>[76.6-76.73]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[84.11-84.22]</c:v>
+                  <c:v>[76.73-76.86]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[84.22-84.33]</c:v>
+                  <c:v>[76.86-76.99]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[84.33-84.44]</c:v>
+                  <c:v>[76.99-77.11]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.44-84.55]</c:v>
+                  <c:v>[77.11-77.24]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.55-84.66]</c:v>
+                  <c:v>[77.24-77.37]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.66-84.77]</c:v>
+                  <c:v>[77.37-77.5]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.77-84.88]</c:v>
+                  <c:v>[77.5-77.63]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.88-84.99]</c:v>
+                  <c:v>[77.63-77.76]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[84.99-85.1]</c:v>
+                  <c:v>[77.76-77.89]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[85.1-85.21]</c:v>
+                  <c:v>[77.89-78.02]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2235,46 +2232,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2412,28 +2409,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>34</c:v>
@@ -2451,28 +2448,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2600,31 +2597,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2639,28 +2636,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2788,31 +2785,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2827,25 +2824,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2</c:v>
@@ -2975,46 +2972,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.7924-3.8222]</c:v>
+                  <c:v>[3.345-3.362]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.8222-3.852]</c:v>
+                  <c:v>[3.362-3.38]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.852-3.8817]</c:v>
+                  <c:v>[3.38-3.397]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.8817-3.9115]</c:v>
+                  <c:v>[3.397-3.414]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.9115-3.9413]</c:v>
+                  <c:v>[3.414-3.432]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9413-3.971]</c:v>
+                  <c:v>[3.432-3.449]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.971-4.0008]</c:v>
+                  <c:v>[3.449-3.467]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.0008-4.0306]</c:v>
+                  <c:v>[3.467-3.484]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.0306-4.0603]</c:v>
+                  <c:v>[3.484-3.501]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.0603-4.0901]</c:v>
+                  <c:v>[3.501-3.519]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.0901-4.1199]</c:v>
+                  <c:v>[3.519-3.536]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.1199-4.1496]</c:v>
+                  <c:v>[3.536-3.554]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.1496-4.1794]</c:v>
+                  <c:v>[3.554-3.571]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.1794-4.2092]</c:v>
+                  <c:v>[3.571-3.588]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3026,43 +3023,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>15</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -3202,46 +3199,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.8259-3.8431]</c:v>
+                  <c:v>[3.345-3.356]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.8431-3.8603]</c:v>
+                  <c:v>[3.356-3.366]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.8603-3.8776]</c:v>
+                  <c:v>[3.366-3.377]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.8776-3.8948]</c:v>
+                  <c:v>[3.377-3.388]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.8948-3.912]</c:v>
+                  <c:v>[3.388-3.398]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.912-3.9292]</c:v>
+                  <c:v>[3.398-3.409]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.9292-3.9464]</c:v>
+                  <c:v>[3.409-3.42]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.9464-3.9637]</c:v>
+                  <c:v>[3.42-3.43]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.9637-3.9809]</c:v>
+                  <c:v>[3.43-3.441]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.9809-3.9981]</c:v>
+                  <c:v>[3.441-3.452]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.9981-4.0153]</c:v>
+                  <c:v>[3.452-3.463]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.0153-4.0325]</c:v>
+                  <c:v>[3.463-3.473]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.0325-4.0497]</c:v>
+                  <c:v>[3.473-3.484]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.0497-4.067]</c:v>
+                  <c:v>[3.484-3.495]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3256,43 +3253,43 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3429,46 +3426,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.8687-3.893]</c:v>
+                  <c:v>[3.453-3.462]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.893-3.9173]</c:v>
+                  <c:v>[3.462-3.472]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.9173-3.9416]</c:v>
+                  <c:v>[3.472-3.482]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.9416-3.966]</c:v>
+                  <c:v>[3.482-3.492]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.966-3.9903]</c:v>
+                  <c:v>[3.492-3.501]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.9903-4.0146]</c:v>
+                  <c:v>[3.501-3.511]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.0146-4.0389]</c:v>
+                  <c:v>[3.511-3.521]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.0389-4.0633]</c:v>
+                  <c:v>[3.521-3.53]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.0633-4.0876]</c:v>
+                  <c:v>[3.53-3.54]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[4.0876-4.1119]</c:v>
+                  <c:v>[3.54-3.55]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[4.1119-4.1362]</c:v>
+                  <c:v>[3.55-3.559]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[4.1362-4.1605]</c:v>
+                  <c:v>[3.559-3.569]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.1605-4.1849]</c:v>
+                  <c:v>[3.569-3.579]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.1849-4.2092]</c:v>
+                  <c:v>[3.579-3.588]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3480,46 +3477,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3656,46 +3653,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.7924-3.8103]</c:v>
+                  <c:v>[3.353-3.365]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.8103-3.8281]</c:v>
+                  <c:v>[3.365-3.378]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.8281-3.846]</c:v>
+                  <c:v>[3.378-3.39]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.846-3.8639]</c:v>
+                  <c:v>[3.39-3.402]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.8639-3.8817]</c:v>
+                  <c:v>[3.402-3.415]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.8817-3.8996]</c:v>
+                  <c:v>[3.415-3.427]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.8996-3.9175]</c:v>
+                  <c:v>[3.427-3.439]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.9175-3.9353]</c:v>
+                  <c:v>[3.439-3.451]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.9353-3.9532]</c:v>
+                  <c:v>[3.451-3.464]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.9532-3.9711]</c:v>
+                  <c:v>[3.464-3.476]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.9711-3.9889]</c:v>
+                  <c:v>[3.476-3.488]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.9889-4.0068]</c:v>
+                  <c:v>[3.488-3.501]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[4.0068-4.0247]</c:v>
+                  <c:v>[3.501-3.513]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[4.0247-4.0425]</c:v>
+                  <c:v>[3.513-3.525]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3707,40 +3704,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -3883,46 +3880,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[9.255-9.434]</c:v>
+                  <c:v>[11.46-11.53]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[9.434-9.613]</c:v>
+                  <c:v>[11.53-11.6]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[9.613-9.792]</c:v>
+                  <c:v>[11.6-11.67]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[9.792-9.97]</c:v>
+                  <c:v>[11.67-11.74]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[9.97-10.149]</c:v>
+                  <c:v>[11.74-11.81]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[10.149-10.328]</c:v>
+                  <c:v>[11.81-11.87]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.328-10.507]</c:v>
+                  <c:v>[11.87-11.94]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.507-10.685]</c:v>
+                  <c:v>[11.94-12.01]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.685-10.864]</c:v>
+                  <c:v>[12.01-12.08]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.864-11.043]</c:v>
+                  <c:v>[12.08-12.15]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.043-11.222]</c:v>
+                  <c:v>[12.15-12.22]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.222-11.4]</c:v>
+                  <c:v>[12.22-12.29]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.4-11.579]</c:v>
+                  <c:v>[12.29-12.35]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.579-11.758]</c:v>
+                  <c:v>[12.35-12.42]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3937,43 +3934,43 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>17</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4923,7 +4920,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -4931,71 +4928,71 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>115</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>83</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>47</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -5017,7 +5014,7 @@
         <v>70</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5025,7 +5022,7 @@
         <v>71</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5033,7 +5030,7 @@
         <v>72</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5041,7 +5038,7 @@
         <v>73</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5049,7 +5046,7 @@
         <v>74</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5057,7 +5054,7 @@
         <v>75</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5065,7 +5062,7 @@
         <v>76</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5073,7 +5070,7 @@
         <v>77</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5081,7 +5078,7 @@
         <v>78</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5089,7 +5086,7 @@
         <v>79</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5097,7 +5094,7 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5105,7 +5102,7 @@
         <v>81</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5113,7 +5110,7 @@
         <v>82</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5121,7 +5118,7 @@
         <v>83</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5143,7 +5140,7 @@
         <v>84</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5151,7 +5148,7 @@
         <v>85</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5159,7 +5156,7 @@
         <v>86</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5167,7 +5164,7 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5175,7 +5172,7 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5183,7 +5180,7 @@
         <v>89</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5191,7 +5188,7 @@
         <v>90</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5199,7 +5196,7 @@
         <v>91</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5207,7 +5204,7 @@
         <v>92</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5215,7 +5212,7 @@
         <v>93</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5223,7 +5220,7 @@
         <v>94</v>
       </c>
       <c r="B11">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5231,7 +5228,7 @@
         <v>95</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5239,7 +5236,7 @@
         <v>96</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5247,7 +5244,7 @@
         <v>97</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5285,20 +5282,20 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -5306,74 +5303,74 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5392,114 +5389,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B10">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11">
-        <v>57</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5518,15 +5515,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -5534,15 +5531,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5550,82 +5547,82 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B11">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5644,114 +5641,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5770,23 +5767,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5794,71 +5791,71 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -5866,18 +5863,18 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5896,7 +5893,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5904,55 +5901,55 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5963,7 +5960,7 @@
         <v>34</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5987,7 +5984,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5995,31 +5992,31 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6027,39 +6024,39 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -6078,7 +6075,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6086,63 +6083,63 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B3">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -6150,7 +6147,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -6172,7 +6169,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6180,7 +6177,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6188,7 +6185,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6196,7 +6193,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>51</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6204,7 +6201,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6212,7 +6209,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6220,7 +6217,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6228,7 +6225,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6236,7 +6233,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6244,7 +6241,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6252,7 +6249,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6260,7 +6257,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6268,7 +6265,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6306,7 +6303,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6314,7 +6311,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6322,7 +6319,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6330,7 +6327,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6338,7 +6335,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6346,7 +6343,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6354,7 +6351,7 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6362,7 +6359,7 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6370,7 +6367,7 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6378,7 +6375,7 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6386,7 +6383,7 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6394,7 +6391,7 @@
         <v>26</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6402,7 +6399,7 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6424,7 +6421,7 @@
         <v>28</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6432,7 +6429,7 @@
         <v>29</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6440,7 +6437,7 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6448,7 +6445,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6456,7 +6453,7 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6464,7 +6461,7 @@
         <v>33</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6472,7 +6469,7 @@
         <v>34</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6480,7 +6477,7 @@
         <v>35</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6488,7 +6485,7 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6496,7 +6493,7 @@
         <v>37</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6504,7 +6501,7 @@
         <v>38</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6512,7 +6509,7 @@
         <v>39</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6520,7 +6517,7 @@
         <v>40</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6528,7 +6525,7 @@
         <v>41</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6550,7 +6547,7 @@
         <v>42</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6558,7 +6555,7 @@
         <v>43</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6566,7 +6563,7 @@
         <v>44</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6574,7 +6571,7 @@
         <v>45</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6582,7 +6579,7 @@
         <v>46</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6590,7 +6587,7 @@
         <v>47</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6598,7 +6595,7 @@
         <v>48</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6606,7 +6603,7 @@
         <v>49</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6614,7 +6611,7 @@
         <v>50</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6622,7 +6619,7 @@
         <v>51</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6630,7 +6627,7 @@
         <v>52</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6638,7 +6635,7 @@
         <v>53</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6684,7 +6681,7 @@
         <v>57</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6692,7 +6689,7 @@
         <v>58</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6700,7 +6697,7 @@
         <v>59</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6708,7 +6705,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6716,7 +6713,7 @@
         <v>61</v>
       </c>
       <c r="B6">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6724,7 +6721,7 @@
         <v>62</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6732,7 +6729,7 @@
         <v>63</v>
       </c>
       <c r="B8">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6740,7 +6737,7 @@
         <v>64</v>
       </c>
       <c r="B9">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6748,7 +6745,7 @@
         <v>65</v>
       </c>
       <c r="B10">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6756,7 +6753,7 @@
         <v>66</v>
       </c>
       <c r="B11">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6764,7 +6761,7 @@
         <v>67</v>
       </c>
       <c r="B12">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6772,7 +6769,7 @@
         <v>68</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6780,7 +6777,7 @@
         <v>69</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>